<commit_message>
Industry temporal profile, Energy updated
</commit_message>
<xml_diff>
--- a/Datasets_summary.xlsx
+++ b/Datasets_summary.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R_projects\Spatialization\"/>
@@ -16,7 +16,7 @@
     <sheet name="Temporal distrib. - methodology" sheetId="2" r:id="rId2"/>
     <sheet name="Temporal distribution - summary" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1021,7 +1021,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6671,11 +6671,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA239"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16041,7 +16041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
       <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Other prcesses temporal profile
</commit_message>
<xml_diff>
--- a/Datasets_summary.xlsx
+++ b/Datasets_summary.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="297">
   <si>
     <t>NFR category</t>
   </si>
@@ -591,9 +591,6 @@
     <t>HE = WD + WT0816 + WT1624 + WW + !PH + !RP</t>
   </si>
   <si>
-    <t>HE = WDWW + WT0816 + WT1624 + !PH + SA</t>
-  </si>
-  <si>
     <t>Vehicles trend  activity (VA)</t>
   </si>
   <si>
@@ -604,12 +601,6 @@
   </si>
   <si>
     <t>HE = WD + WT0816 + DL + WE +  !PH + SA</t>
-  </si>
-  <si>
-    <t>HE = WDWW + WT0816 + !PH + VA</t>
-  </si>
-  <si>
-    <t>HE = WDWW + WT0024 + SA + TEMP + SLP</t>
   </si>
   <si>
     <t>Number of flights per hour (NFH)</t>
@@ -796,27 +787,6 @@
     <t>The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the coating applications happens during the whole year, proportionally to the road activity, but with the less activity during the nigth and public holidays. The activity graph will be constructed by assuming that the road activity is higher by day light, for the working days, for the rush hours.</t>
   </si>
   <si>
-    <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the domestic solvent use including fungicides happens during the whole year, but with the less activity during the nigth. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
-  </si>
-  <si>
-    <t>HE = WDWW + DL + TEMP + SLP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the degreasing happens during the whole year, but with the less activity during the nigth. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the dry cleaning happens during the whole year, but with the less activity during the nigth. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the emission from using chemical products happens during the whole year, but with the less activity during the nigth. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the emission from printing happens during the whole year, but with the less activity during the nigth. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the emissions from other solvent and product use happens during the whole year, but with the less activity during the nigth. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
-  </si>
-  <si>
     <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph was constructed by assuming that wood processing  happens during the whole year at working days, but with less activity during the night, weekends and public holidays as well as during the extreme winter.  </t>
   </si>
   <si>
@@ -835,13 +805,7 @@
     <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that emission  happens during the whole year, but with the less activity during the nigth as well as during the extreme winter. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
   </si>
   <si>
-    <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the biological treatment of waste - solid waste disposal on land happens during the whole year, proportionally to the road activity, but with the less activity during the nigth and public holidays. </t>
-  </si>
-  <si>
     <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the cremation happens during the whole year, but with the less activity during the nigth and public holidays. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the domestic wastewater handling happens during the whole year, but with the less activity during the public holidays as well as during the extreme winter. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
   </si>
   <si>
     <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the industrial wastewater handling  happens during the whole year, but with the less activity during the public holidays as well as during the extreme winter. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
@@ -1016,6 +980,51 @@
   </si>
   <si>
     <t>HE = WDWW + (k+DL) + (k+SAAG) + inverse(TEMP) + SLP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HE = WDWW + WT0816 + !PH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the biological treatment of waste - solid waste disposal on land happens during the whole year, but with the less activity during the nigth and public holidays. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the domestic wastewater handling happens during the whole year, but with the less activity during the public holidays. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
+  </si>
+  <si>
+    <t>HE = WDWW + WT0024  + TEMP + SLP</t>
+  </si>
+  <si>
+    <t>HE = WDWW + WT0024 + TEMP + SLP</t>
+  </si>
+  <si>
+    <t>Working time for heating season [06-22h] (WT0622)</t>
+  </si>
+  <si>
+    <t>HE = WDWW + WT0024 + !PH + (k1*SA + k2) + !RP</t>
+  </si>
+  <si>
+    <t>HE = WDWW + WT0816 + WT1624 + !PH + (k1*SA + k2)</t>
+  </si>
+  <si>
+    <t>HE = WDWW + DL + inverse(TEMP) + SLP + !PH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the domestic solvent use including fungicides happens during the whole year, but with the less activity during the nigth and public holidays. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the degreasing happens during the whole year, but with the less activity during the nigth and public holidays. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the dry cleaning happens during the whole year, but with the less activity during the nigth and public holidays. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the emission from using chemical products happens during the whole year, but with the less activity during the nigth and public holidays. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the emission from printing happens during the whole year, but with the less activity during the nigth and public holidays. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the emissions from other solvent and product use happens during the whole year, but with the less activity during the nigth and public holidays. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
   </si>
 </sst>
 </file>
@@ -4224,7 +4233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -6671,11 +6680,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA239"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X63" sqref="X63"/>
+      <selection pane="bottomRight" activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6706,7 +6715,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="245" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G1" s="246"/>
       <c r="H1" s="246"/>
@@ -6739,7 +6748,7 @@
         <v>148</v>
       </c>
       <c r="D2" s="110" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E2" s="111" t="s">
         <v>115</v>
@@ -6760,7 +6769,7 @@
         <v>168</v>
       </c>
       <c r="K2" s="113" t="s">
-        <v>166</v>
+        <v>287</v>
       </c>
       <c r="L2" s="113" t="s">
         <v>153</v>
@@ -6796,10 +6805,10 @@
         <v>161</v>
       </c>
       <c r="W2" s="161" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="X2" s="161" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="Y2" s="114" t="s">
         <v>162</v>
@@ -6819,13 +6828,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="134" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D3" s="134" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E3" s="187" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F3" s="135" t="s">
         <v>164</v>
@@ -6901,10 +6910,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E4" s="116"/>
       <c r="F4" s="123" t="s">
@@ -6968,7 +6977,7 @@
         <v>138</v>
       </c>
       <c r="Z4" s="147" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="AA4" s="122">
         <f t="shared" si="0"/>
@@ -6981,7 +6990,7 @@
         <v>68</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D5" s="194"/>
       <c r="E5" s="116"/>
@@ -7046,7 +7055,7 @@
         <v>138</v>
       </c>
       <c r="Z5" s="147" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="AA5" s="122">
         <f t="shared" si="0"/>
@@ -7059,7 +7068,7 @@
         <v>69</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D6" s="194"/>
       <c r="E6" s="116"/>
@@ -7124,7 +7133,7 @@
         <v>138</v>
       </c>
       <c r="Z6" s="147" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="AA6" s="122">
         <f t="shared" si="0"/>
@@ -7137,7 +7146,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D7" s="194"/>
       <c r="E7" s="150" t="s">
@@ -7217,7 +7226,7 @@
         <v>70</v>
       </c>
       <c r="C8" s="153" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D8" s="195"/>
       <c r="E8" s="165" t="s">
@@ -7299,7 +7308,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="134" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D9" s="196"/>
       <c r="E9" s="117"/>
@@ -7377,7 +7386,7 @@
         <v>75</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D10" s="194"/>
       <c r="E10" s="116"/>
@@ -7442,7 +7451,7 @@
         <v>164</v>
       </c>
       <c r="Z10" s="163" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="AA10" s="144">
         <f t="shared" si="0"/>
@@ -7455,7 +7464,7 @@
         <v>111</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="D11" s="194"/>
       <c r="E11" s="116"/>
@@ -7520,7 +7529,7 @@
         <v>164</v>
       </c>
       <c r="Z11" s="163" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AA11" s="144">
         <f t="shared" si="0"/>
@@ -7533,7 +7542,7 @@
         <v>76</v>
       </c>
       <c r="C12" s="153" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D12" s="195"/>
       <c r="E12" s="129"/>
@@ -7541,7 +7550,7 @@
         <v>164</v>
       </c>
       <c r="G12" s="130" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H12" s="130" t="s">
         <v>164</v>
@@ -7550,7 +7559,7 @@
         <v>164</v>
       </c>
       <c r="J12" s="130" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K12" s="130" t="s">
         <v>164</v>
@@ -7598,7 +7607,7 @@
         <v>164</v>
       </c>
       <c r="Z12" s="166" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AA12" s="160">
         <f t="shared" si="0"/>
@@ -7613,7 +7622,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="134" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="D13" s="134"/>
       <c r="E13" s="117"/>
@@ -7678,7 +7687,7 @@
         <v>164</v>
       </c>
       <c r="Z13" s="140" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="AA13" s="143">
         <f t="shared" si="0"/>
@@ -7691,7 +7700,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D14" s="194"/>
       <c r="E14" s="116"/>
@@ -7756,7 +7765,7 @@
         <v>164</v>
       </c>
       <c r="Z14" s="141" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AA14" s="144">
         <f t="shared" si="0"/>
@@ -7769,7 +7778,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D15" s="194"/>
       <c r="E15" s="116"/>
@@ -7834,7 +7843,7 @@
         <v>164</v>
       </c>
       <c r="Z15" s="141" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="AA15" s="144">
         <f t="shared" si="0"/>
@@ -7847,7 +7856,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D16" s="194"/>
       <c r="E16" s="116"/>
@@ -7912,7 +7921,7 @@
         <v>164</v>
       </c>
       <c r="Z16" s="141" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="AA16" s="144">
         <f t="shared" si="0"/>
@@ -7925,7 +7934,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D17" s="194"/>
       <c r="E17" s="116"/>
@@ -7990,7 +7999,7 @@
         <v>164</v>
       </c>
       <c r="Z17" s="141" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="AA17" s="144">
         <f t="shared" si="0"/>
@@ -8003,7 +8012,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D18" s="194"/>
       <c r="E18" s="116"/>
@@ -8068,7 +8077,7 @@
         <v>164</v>
       </c>
       <c r="Z18" s="141" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="AA18" s="144">
         <f t="shared" si="0"/>
@@ -8081,7 +8090,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D19" s="194"/>
       <c r="E19" s="116"/>
@@ -8146,7 +8155,7 @@
         <v>164</v>
       </c>
       <c r="Z19" s="141" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="AA19" s="144">
         <f t="shared" si="0"/>
@@ -8159,7 +8168,7 @@
         <v>15</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D20" s="194"/>
       <c r="E20" s="116"/>
@@ -8224,7 +8233,7 @@
         <v>164</v>
       </c>
       <c r="Z20" s="141" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="AA20" s="144">
         <f t="shared" si="0"/>
@@ -8237,7 +8246,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D21" s="194"/>
       <c r="E21" s="116"/>
@@ -8302,7 +8311,7 @@
         <v>164</v>
       </c>
       <c r="Z21" s="141" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="AA21" s="144">
         <f t="shared" si="0"/>
@@ -8315,7 +8324,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D22" s="194"/>
       <c r="E22" s="116"/>
@@ -8380,7 +8389,7 @@
         <v>164</v>
       </c>
       <c r="Z22" s="141" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="AA22" s="144">
         <f t="shared" si="0"/>
@@ -8393,7 +8402,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D23" s="194"/>
       <c r="E23" s="116"/>
@@ -8458,7 +8467,7 @@
         <v>164</v>
       </c>
       <c r="Z23" s="141" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AA23" s="144">
         <f t="shared" si="0"/>
@@ -8471,7 +8480,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="153" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D24" s="195"/>
       <c r="E24" s="129"/>
@@ -8536,7 +8545,7 @@
         <v>164</v>
       </c>
       <c r="Z24" s="142" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AA24" s="145">
         <f t="shared" si="0"/>
@@ -8551,7 +8560,7 @@
         <v>91</v>
       </c>
       <c r="C25" s="134" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D25" s="196"/>
       <c r="E25" s="117"/>
@@ -8616,7 +8625,7 @@
         <v>164</v>
       </c>
       <c r="Z25" s="184" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="AA25" s="176">
         <f t="shared" si="0"/>
@@ -8629,7 +8638,7 @@
         <v>93</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D26" s="194"/>
       <c r="E26" s="116"/>
@@ -8694,7 +8703,7 @@
         <v>164</v>
       </c>
       <c r="Z26" s="163" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="AA26" s="144">
         <f t="shared" si="0"/>
@@ -8707,7 +8716,7 @@
         <v>92</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="D27" s="194"/>
       <c r="E27" s="116"/>
@@ -8785,7 +8794,7 @@
         <v>21</v>
       </c>
       <c r="C28" s="153" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D28" s="195"/>
       <c r="E28" s="129"/>
@@ -8865,7 +8874,7 @@
         <v>23</v>
       </c>
       <c r="C29" s="134" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D29" s="117"/>
       <c r="E29" s="117"/>
@@ -8943,7 +8952,7 @@
         <v>104</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D30" s="116"/>
       <c r="E30" s="116"/>
@@ -9021,7 +9030,7 @@
         <v>106</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D31" s="116"/>
       <c r="E31" s="116"/>
@@ -9099,7 +9108,7 @@
         <v>105</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D32" s="116"/>
       <c r="E32" s="116"/>
@@ -9177,7 +9186,7 @@
         <v>107</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D33" s="116"/>
       <c r="E33" s="116"/>
@@ -9255,7 +9264,7 @@
         <v>109</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D34" s="116"/>
       <c r="E34" s="116"/>
@@ -9333,7 +9342,7 @@
         <v>24</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D35" s="116"/>
       <c r="E35" s="116"/>
@@ -9411,7 +9420,7 @@
         <v>25</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D36" s="116"/>
       <c r="E36" s="116"/>
@@ -9489,7 +9498,7 @@
         <v>26</v>
       </c>
       <c r="C37" s="137" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D37" s="118"/>
       <c r="E37" s="118"/>
@@ -9569,7 +9578,7 @@
         <v>27</v>
       </c>
       <c r="C38" s="189" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D38" s="190"/>
       <c r="E38" s="190"/>
@@ -9634,7 +9643,7 @@
         <v>138</v>
       </c>
       <c r="Z38" s="162" t="s">
-        <v>174</v>
+        <v>288</v>
       </c>
       <c r="AA38" s="143">
         <f t="shared" si="1"/>
@@ -9647,7 +9656,7 @@
         <v>28</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D39" s="116"/>
       <c r="E39" s="116"/>
@@ -9712,7 +9721,7 @@
         <v>164</v>
       </c>
       <c r="Z39" s="163" t="s">
-        <v>178</v>
+        <v>289</v>
       </c>
       <c r="AA39" s="144">
         <f t="shared" si="1"/>
@@ -9725,7 +9734,7 @@
         <v>29</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D40" s="116"/>
       <c r="E40" s="116"/>
@@ -9790,7 +9799,7 @@
         <v>164</v>
       </c>
       <c r="Z40" s="163" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AA40" s="144">
         <f t="shared" si="1"/>
@@ -9803,7 +9812,7 @@
         <v>30</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>231</v>
+        <v>291</v>
       </c>
       <c r="D41" s="116"/>
       <c r="E41" s="116"/>
@@ -9841,7 +9850,7 @@
         <v>164</v>
       </c>
       <c r="Q41" s="123" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="R41" s="123" t="s">
         <v>164</v>
@@ -9868,11 +9877,11 @@
         <v>164</v>
       </c>
       <c r="Z41" s="163" t="s">
-        <v>232</v>
+        <v>290</v>
       </c>
       <c r="AA41" s="144">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -9881,7 +9890,7 @@
         <v>31</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D42" s="116"/>
       <c r="E42" s="116"/>
@@ -9946,7 +9955,7 @@
         <v>164</v>
       </c>
       <c r="Z42" s="163" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AA42" s="144">
         <f t="shared" si="1"/>
@@ -9959,7 +9968,7 @@
         <v>32</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D43" s="116"/>
       <c r="E43" s="116"/>
@@ -10024,7 +10033,7 @@
         <v>164</v>
       </c>
       <c r="Z43" s="163" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AA43" s="144">
         <f t="shared" si="1"/>
@@ -10037,7 +10046,7 @@
         <v>33</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D44" s="116"/>
       <c r="E44" s="116"/>
@@ -10102,7 +10111,7 @@
         <v>164</v>
       </c>
       <c r="Z44" s="163" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AA44" s="144">
         <f t="shared" si="1"/>
@@ -10115,7 +10124,7 @@
         <v>34</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>233</v>
+        <v>292</v>
       </c>
       <c r="D45" s="116"/>
       <c r="E45" s="116"/>
@@ -10153,7 +10162,7 @@
         <v>164</v>
       </c>
       <c r="Q45" s="123" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="R45" s="123" t="s">
         <v>164</v>
@@ -10180,11 +10189,11 @@
         <v>164</v>
       </c>
       <c r="Z45" s="163" t="s">
-        <v>232</v>
+        <v>290</v>
       </c>
       <c r="AA45" s="144">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -10193,7 +10202,7 @@
         <v>35</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>234</v>
+        <v>293</v>
       </c>
       <c r="D46" s="116"/>
       <c r="E46" s="116"/>
@@ -10231,7 +10240,7 @@
         <v>164</v>
       </c>
       <c r="Q46" s="123" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="R46" s="123" t="s">
         <v>164</v>
@@ -10258,11 +10267,11 @@
         <v>164</v>
       </c>
       <c r="Z46" s="163" t="s">
-        <v>232</v>
+        <v>290</v>
       </c>
       <c r="AA46" s="144">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -10271,7 +10280,7 @@
         <v>36</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>235</v>
+        <v>294</v>
       </c>
       <c r="D47" s="116"/>
       <c r="E47" s="116"/>
@@ -10309,7 +10318,7 @@
         <v>164</v>
       </c>
       <c r="Q47" s="123" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="R47" s="123" t="s">
         <v>164</v>
@@ -10336,11 +10345,11 @@
         <v>164</v>
       </c>
       <c r="Z47" s="163" t="s">
-        <v>232</v>
+        <v>290</v>
       </c>
       <c r="AA47" s="144">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -10349,7 +10358,7 @@
         <v>37</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>236</v>
+        <v>295</v>
       </c>
       <c r="D48" s="116"/>
       <c r="E48" s="116"/>
@@ -10387,7 +10396,7 @@
         <v>164</v>
       </c>
       <c r="Q48" s="123" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="R48" s="123" t="s">
         <v>164</v>
@@ -10414,11 +10423,11 @@
         <v>164</v>
       </c>
       <c r="Z48" s="163" t="s">
-        <v>232</v>
+        <v>290</v>
       </c>
       <c r="AA48" s="144">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -10427,7 +10436,7 @@
         <v>120</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>237</v>
+        <v>296</v>
       </c>
       <c r="D49" s="116"/>
       <c r="E49" s="116"/>
@@ -10465,7 +10474,7 @@
         <v>164</v>
       </c>
       <c r="Q49" s="123" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="R49" s="123" t="s">
         <v>164</v>
@@ -10492,11 +10501,11 @@
         <v>164</v>
       </c>
       <c r="Z49" s="163" t="s">
-        <v>232</v>
+        <v>290</v>
       </c>
       <c r="AA49" s="144">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:27" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10505,7 +10514,7 @@
         <v>38</v>
       </c>
       <c r="C50" s="153" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D50" s="129"/>
       <c r="E50" s="129"/>
@@ -10570,7 +10579,7 @@
         <v>164</v>
       </c>
       <c r="Z50" s="166" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AA50" s="160">
         <f t="shared" si="1"/>
@@ -10585,7 +10594,7 @@
         <v>40</v>
       </c>
       <c r="C51" s="134" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="D51" s="117"/>
       <c r="E51" s="117"/>
@@ -10650,7 +10659,7 @@
         <v>164</v>
       </c>
       <c r="Z51" s="162" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="AA51" s="143">
         <f t="shared" si="1"/>
@@ -10663,7 +10672,7 @@
         <v>41</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D52" s="116"/>
       <c r="E52" s="116"/>
@@ -10728,7 +10737,7 @@
         <v>164</v>
       </c>
       <c r="Z52" s="163" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="AA52" s="144">
         <f t="shared" si="1"/>
@@ -10741,7 +10750,7 @@
         <v>42</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D53" s="116"/>
       <c r="E53" s="116"/>
@@ -10806,7 +10815,7 @@
         <v>164</v>
       </c>
       <c r="Z53" s="163" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="AA53" s="144">
         <f t="shared" si="1"/>
@@ -10819,7 +10828,7 @@
         <v>43</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D54" s="116"/>
       <c r="E54" s="116"/>
@@ -10884,7 +10893,7 @@
         <v>164</v>
       </c>
       <c r="Z54" s="163" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="AA54" s="144">
         <f t="shared" si="1"/>
@@ -10897,7 +10906,7 @@
         <v>44</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D55" s="116"/>
       <c r="E55" s="116"/>
@@ -10962,7 +10971,7 @@
         <v>164</v>
       </c>
       <c r="Z55" s="163" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="AA55" s="144">
         <f t="shared" si="1"/>
@@ -10975,7 +10984,7 @@
         <v>45</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D56" s="116"/>
       <c r="E56" s="116"/>
@@ -11040,7 +11049,7 @@
         <v>164</v>
       </c>
       <c r="Z56" s="163" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="AA56" s="144">
         <f t="shared" si="1"/>
@@ -11053,7 +11062,7 @@
         <v>46</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D57" s="116"/>
       <c r="E57" s="116"/>
@@ -11118,7 +11127,7 @@
         <v>164</v>
       </c>
       <c r="Z57" s="163" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="AA57" s="144">
         <f t="shared" si="1"/>
@@ -11131,7 +11140,7 @@
         <v>47</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D58" s="116"/>
       <c r="E58" s="116"/>
@@ -11196,7 +11205,7 @@
         <v>164</v>
       </c>
       <c r="Z58" s="163" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="AA58" s="144">
         <f t="shared" si="1"/>
@@ -11209,7 +11218,7 @@
         <v>48</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D59" s="116"/>
       <c r="E59" s="116"/>
@@ -11274,7 +11283,7 @@
         <v>164</v>
       </c>
       <c r="Z59" s="163" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="AA59" s="144">
         <f t="shared" si="1"/>
@@ -11287,7 +11296,7 @@
         <v>49</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="D60" s="116"/>
       <c r="E60" s="116"/>
@@ -11348,7 +11357,7 @@
         <v>164</v>
       </c>
       <c r="Z60" s="163" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="AA60" s="144">
         <f t="shared" si="1"/>
@@ -11361,7 +11370,7 @@
         <v>50</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="D61" s="116"/>
       <c r="E61" s="116"/>
@@ -11422,7 +11431,7 @@
         <v>164</v>
       </c>
       <c r="Z61" s="163" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="AA61" s="144">
         <f t="shared" si="1"/>
@@ -11435,7 +11444,7 @@
         <v>51</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D62" s="116"/>
       <c r="E62" s="116"/>
@@ -11500,7 +11509,7 @@
         <v>164</v>
       </c>
       <c r="Z62" s="163" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="AA62" s="144">
         <f t="shared" si="1"/>
@@ -11513,7 +11522,7 @@
         <v>52</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D63" s="116"/>
       <c r="E63" s="116"/>
@@ -11578,7 +11587,7 @@
         <v>164</v>
       </c>
       <c r="Z63" s="163" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="AA63" s="144">
         <f t="shared" si="1"/>
@@ -11591,7 +11600,7 @@
         <v>53</v>
       </c>
       <c r="C64" s="153" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="D64" s="129"/>
       <c r="E64" s="129"/>
@@ -11656,7 +11665,7 @@
         <v>164</v>
       </c>
       <c r="Z64" s="152" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="AA64" s="145">
         <f t="shared" si="1"/>
@@ -11671,7 +11680,7 @@
         <v>55</v>
       </c>
       <c r="C65" s="134" t="s">
-        <v>244</v>
+        <v>283</v>
       </c>
       <c r="D65" s="117"/>
       <c r="E65" s="117"/>
@@ -11727,7 +11736,7 @@
         <v>164</v>
       </c>
       <c r="W65" s="135" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="X65" s="135" t="s">
         <v>164</v>
@@ -11736,11 +11745,11 @@
         <v>164</v>
       </c>
       <c r="Z65" s="184" t="s">
-        <v>183</v>
+        <v>282</v>
       </c>
       <c r="AA65" s="176">
         <f>COUNTIF(G65:Y65,"X")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -11749,7 +11758,7 @@
         <v>56</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="D66" s="116"/>
       <c r="E66" s="116"/>
@@ -11814,7 +11823,7 @@
         <v>164</v>
       </c>
       <c r="Z66" s="163" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="AA66" s="144">
         <f>COUNTIF(F66:Y66,"X")</f>
@@ -11827,7 +11836,7 @@
         <v>57</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>246</v>
+        <v>284</v>
       </c>
       <c r="D67" s="116"/>
       <c r="E67" s="116"/>
@@ -11868,7 +11877,7 @@
         <v>164</v>
       </c>
       <c r="R67" s="123" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="S67" s="123" t="s">
         <v>164</v>
@@ -11892,11 +11901,11 @@
         <v>164</v>
       </c>
       <c r="Z67" s="163" t="s">
-        <v>184</v>
+        <v>285</v>
       </c>
       <c r="AA67" s="144">
         <f>COUNTIF(F67:Y67,"X")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:27" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -11905,7 +11914,7 @@
         <v>58</v>
       </c>
       <c r="C68" s="137" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="D68" s="118"/>
       <c r="E68" s="118"/>
@@ -11946,7 +11955,7 @@
         <v>164</v>
       </c>
       <c r="R68" s="126" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="S68" s="126" t="s">
         <v>164</v>
@@ -11970,11 +11979,11 @@
         <v>164</v>
       </c>
       <c r="Z68" s="152" t="s">
-        <v>184</v>
+        <v>286</v>
       </c>
       <c r="AA68" s="145">
         <f>COUNTIF(F68:Y68,"X")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12027,11 +12036,11 @@
       </c>
       <c r="Q69" s="179">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="R69" s="179">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="S69" s="179">
         <f t="shared" si="2"/>
@@ -12051,7 +12060,7 @@
       </c>
       <c r="W69" s="179">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X69" s="179">
         <f t="shared" si="2"/>
@@ -12063,11 +12072,11 @@
       </c>
       <c r="Z69" s="177">
         <f>SUM(F69:Y69)</f>
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="AA69" s="177">
         <f>SUM(AA3:AA68)</f>
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.25">
@@ -16041,7 +16050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
@@ -16058,19 +16067,19 @@
   <sheetData>
     <row r="1" spans="1:23" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="121" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="B1" s="197" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C1" s="198" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D1" s="198" t="s">
         <v>149</v>
       </c>
       <c r="E1" s="198" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="F1" s="198" t="s">
         <v>61</v>
@@ -16079,7 +16088,7 @@
         <v>115</v>
       </c>
       <c r="H1" s="199" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I1" s="186"/>
       <c r="J1" s="186"/>
@@ -16102,22 +16111,22 @@
         <v>150</v>
       </c>
       <c r="B2" s="134" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="C2" s="204" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="D2" s="204" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E2" s="134" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="F2" s="134">
         <v>2015</v>
       </c>
       <c r="G2" s="187" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="H2" s="205"/>
     </row>
@@ -16126,13 +16135,13 @@
         <v>169</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="C3" s="200" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="D3" s="200" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11">
@@ -16146,13 +16155,13 @@
         <v>151</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="C4" s="200" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D4" s="200" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11">
@@ -16166,13 +16175,13 @@
         <v>152</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="C5" s="200" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D5" s="200" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11">
@@ -16186,13 +16195,13 @@
         <v>168</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="C6" s="200" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D6" s="200" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11">
@@ -16206,22 +16215,22 @@
         <v>166</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="C7" s="200" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D7" s="200" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="F7" s="11">
         <v>2015</v>
       </c>
       <c r="G7" s="212" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="H7" s="207"/>
     </row>
@@ -16230,22 +16239,22 @@
         <v>153</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C8" s="200" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D8" s="200" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F8" s="11">
         <v>2015</v>
       </c>
       <c r="G8" s="150" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H8" s="207"/>
     </row>
@@ -16254,13 +16263,13 @@
         <v>154</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="C9" s="200" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="D9" s="200" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="1">
@@ -16274,13 +16283,13 @@
         <v>175</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="C10" s="200" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D10" s="200" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="1">
@@ -16294,13 +16303,13 @@
         <v>155</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="C11" s="200" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D11" s="200" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="1">
@@ -16314,13 +16323,13 @@
         <v>156</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="C12" s="200" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D12" s="200" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="E12" s="153"/>
       <c r="F12" s="1">
@@ -16334,22 +16343,22 @@
         <v>157</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="C13" s="200" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="D13" s="200" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="F13" s="1">
         <v>2015</v>
       </c>
       <c r="G13" s="212" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="H13" s="207"/>
     </row>
@@ -16358,22 +16367,22 @@
         <v>158</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C14" s="200" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="D14" s="200" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F14" s="11">
         <v>2015</v>
       </c>
       <c r="G14" s="150" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H14" s="207"/>
     </row>
@@ -16382,22 +16391,22 @@
         <v>165</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="C15" s="200" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="D15" s="200" t="s">
+        <v>255</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>267</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>279</v>
       </c>
       <c r="F15" s="11">
         <v>2015</v>
       </c>
       <c r="G15" s="212" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="H15" s="207"/>
     </row>
@@ -16406,13 +16415,13 @@
         <v>159</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="C16" s="200" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="D16" s="200" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="1">
@@ -16426,22 +16435,22 @@
         <v>160</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="C17" s="200" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="D17" s="200" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="F17" s="1">
         <v>2015</v>
       </c>
       <c r="G17" s="150" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="H17" s="207"/>
     </row>
@@ -16450,40 +16459,40 @@
         <v>161</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="C18" s="200" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="D18" s="200" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="F18" s="1">
         <v>2015</v>
       </c>
       <c r="G18" s="150" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="H18" s="207"/>
     </row>
     <row r="19" spans="1:8" ht="408.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="206" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="C19" s="200" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="D19" s="200" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E19" s="153" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="F19" s="11">
         <v>2015</v>
@@ -16493,16 +16502,16 @@
     </row>
     <row r="20" spans="1:8" ht="408.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="206" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="C20" s="200" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D20" s="200" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="1">
@@ -16516,13 +16525,13 @@
         <v>162</v>
       </c>
       <c r="B21" s="137" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="C21" s="209" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="D21" s="209" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="E21" s="137"/>
       <c r="F21" s="210">
@@ -16534,7 +16543,7 @@
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="273" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="B26" s="274"/>
       <c r="C26" s="275"/>
@@ -16542,7 +16551,7 @@
     </row>
     <row r="27" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="272" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="B27" s="272"/>
       <c r="C27" s="272"/>

</xml_diff>

<commit_message>
Fugitive emissions temporal profile
</commit_message>
<xml_diff>
--- a/Datasets_summary.xlsx
+++ b/Datasets_summary.xlsx
@@ -719,9 +719,6 @@
   </si>
   <si>
     <t>The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the exploration, production, transport of liquid fuels happens during the whole year, proportionally to the road activity, but with the less activity during the nigth and public holidays.</t>
-  </si>
-  <si>
-    <t>HE = WD + WT0816 + WT1624 + !PH + VA</t>
   </si>
   <si>
     <t>HE = WDWW + WT0024 + !PH</t>
@@ -1025,6 +1022,9 @@
   </si>
   <si>
     <t xml:space="preserve">The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed by assuming that the emissions from other solvent and product use happens during the whole year, but with the less activity during the nigth and public holidays. The activity graph will be constructed also by assuming that with lower temperatures and higher pressure, emission is higher. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HE = WD + WT0816 + WT1624 + !PH </t>
   </si>
 </sst>
 </file>
@@ -6680,11 +6680,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA239"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L50" sqref="L50"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6769,7 +6769,7 @@
         <v>168</v>
       </c>
       <c r="K2" s="113" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L2" s="113" t="s">
         <v>153</v>
@@ -6977,7 +6977,7 @@
         <v>138</v>
       </c>
       <c r="Z4" s="147" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AA4" s="122">
         <f t="shared" si="0"/>
@@ -7055,7 +7055,7 @@
         <v>138</v>
       </c>
       <c r="Z5" s="147" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AA5" s="122">
         <f t="shared" si="0"/>
@@ -7133,7 +7133,7 @@
         <v>138</v>
       </c>
       <c r="Z6" s="147" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AA6" s="122">
         <f t="shared" si="0"/>
@@ -7442,7 +7442,7 @@
         <v>164</v>
       </c>
       <c r="W10" s="123" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="X10" s="123" t="s">
         <v>164</v>
@@ -7451,11 +7451,11 @@
         <v>164</v>
       </c>
       <c r="Z10" s="163" t="s">
-        <v>206</v>
+        <v>296</v>
       </c>
       <c r="AA10" s="144">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -7464,7 +7464,7 @@
         <v>111</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D11" s="194"/>
       <c r="E11" s="116"/>
@@ -7529,7 +7529,7 @@
         <v>164</v>
       </c>
       <c r="Z11" s="163" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA11" s="144">
         <f t="shared" si="0"/>
@@ -7542,7 +7542,7 @@
         <v>76</v>
       </c>
       <c r="C12" s="153" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D12" s="195"/>
       <c r="E12" s="129"/>
@@ -7550,7 +7550,7 @@
         <v>164</v>
       </c>
       <c r="G12" s="130" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H12" s="130" t="s">
         <v>164</v>
@@ -7559,7 +7559,7 @@
         <v>164</v>
       </c>
       <c r="J12" s="130" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K12" s="130" t="s">
         <v>164</v>
@@ -7607,7 +7607,7 @@
         <v>164</v>
       </c>
       <c r="Z12" s="166" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA12" s="160">
         <f t="shared" si="0"/>
@@ -7622,7 +7622,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="134" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D13" s="134"/>
       <c r="E13" s="117"/>
@@ -7687,7 +7687,7 @@
         <v>164</v>
       </c>
       <c r="Z13" s="140" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AA13" s="143">
         <f t="shared" si="0"/>
@@ -7700,7 +7700,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D14" s="194"/>
       <c r="E14" s="116"/>
@@ -7765,7 +7765,7 @@
         <v>164</v>
       </c>
       <c r="Z14" s="141" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AA14" s="144">
         <f t="shared" si="0"/>
@@ -7778,7 +7778,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D15" s="194"/>
       <c r="E15" s="116"/>
@@ -7856,7 +7856,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D16" s="194"/>
       <c r="E16" s="116"/>
@@ -7934,7 +7934,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D17" s="194"/>
       <c r="E17" s="116"/>
@@ -8012,7 +8012,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D18" s="194"/>
       <c r="E18" s="116"/>
@@ -8090,7 +8090,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D19" s="194"/>
       <c r="E19" s="116"/>
@@ -8168,7 +8168,7 @@
         <v>15</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D20" s="194"/>
       <c r="E20" s="116"/>
@@ -8246,7 +8246,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D21" s="194"/>
       <c r="E21" s="116"/>
@@ -8324,7 +8324,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D22" s="194"/>
       <c r="E22" s="116"/>
@@ -8402,7 +8402,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D23" s="194"/>
       <c r="E23" s="116"/>
@@ -8480,7 +8480,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="153" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D24" s="195"/>
       <c r="E24" s="129"/>
@@ -8545,7 +8545,7 @@
         <v>164</v>
       </c>
       <c r="Z24" s="142" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AA24" s="145">
         <f t="shared" si="0"/>
@@ -8560,7 +8560,7 @@
         <v>91</v>
       </c>
       <c r="C25" s="134" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D25" s="196"/>
       <c r="E25" s="117"/>
@@ -8625,7 +8625,7 @@
         <v>164</v>
       </c>
       <c r="Z25" s="184" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AA25" s="176">
         <f t="shared" si="0"/>
@@ -8638,7 +8638,7 @@
         <v>93</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D26" s="194"/>
       <c r="E26" s="116"/>
@@ -8703,7 +8703,7 @@
         <v>164</v>
       </c>
       <c r="Z26" s="163" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AA26" s="144">
         <f t="shared" si="0"/>
@@ -8716,7 +8716,7 @@
         <v>92</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D27" s="194"/>
       <c r="E27" s="116"/>
@@ -8794,7 +8794,7 @@
         <v>21</v>
       </c>
       <c r="C28" s="153" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D28" s="195"/>
       <c r="E28" s="129"/>
@@ -8952,7 +8952,7 @@
         <v>104</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D30" s="116"/>
       <c r="E30" s="116"/>
@@ -9030,7 +9030,7 @@
         <v>106</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D31" s="116"/>
       <c r="E31" s="116"/>
@@ -9108,7 +9108,7 @@
         <v>105</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D32" s="116"/>
       <c r="E32" s="116"/>
@@ -9186,7 +9186,7 @@
         <v>107</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D33" s="116"/>
       <c r="E33" s="116"/>
@@ -9264,7 +9264,7 @@
         <v>109</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D34" s="116"/>
       <c r="E34" s="116"/>
@@ -9342,7 +9342,7 @@
         <v>24</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D35" s="116"/>
       <c r="E35" s="116"/>
@@ -9420,7 +9420,7 @@
         <v>25</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D36" s="116"/>
       <c r="E36" s="116"/>
@@ -9498,7 +9498,7 @@
         <v>26</v>
       </c>
       <c r="C37" s="137" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D37" s="118"/>
       <c r="E37" s="118"/>
@@ -9578,7 +9578,7 @@
         <v>27</v>
       </c>
       <c r="C38" s="189" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D38" s="190"/>
       <c r="E38" s="190"/>
@@ -9643,7 +9643,7 @@
         <v>138</v>
       </c>
       <c r="Z38" s="162" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AA38" s="143">
         <f t="shared" si="1"/>
@@ -9656,7 +9656,7 @@
         <v>28</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D39" s="116"/>
       <c r="E39" s="116"/>
@@ -9721,7 +9721,7 @@
         <v>164</v>
       </c>
       <c r="Z39" s="163" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AA39" s="144">
         <f t="shared" si="1"/>
@@ -9734,7 +9734,7 @@
         <v>29</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D40" s="116"/>
       <c r="E40" s="116"/>
@@ -9812,7 +9812,7 @@
         <v>30</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D41" s="116"/>
       <c r="E41" s="116"/>
@@ -9877,7 +9877,7 @@
         <v>164</v>
       </c>
       <c r="Z41" s="163" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AA41" s="144">
         <f t="shared" si="1"/>
@@ -9890,7 +9890,7 @@
         <v>31</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D42" s="116"/>
       <c r="E42" s="116"/>
@@ -9968,7 +9968,7 @@
         <v>32</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D43" s="116"/>
       <c r="E43" s="116"/>
@@ -10046,7 +10046,7 @@
         <v>33</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D44" s="116"/>
       <c r="E44" s="116"/>
@@ -10124,7 +10124,7 @@
         <v>34</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D45" s="116"/>
       <c r="E45" s="116"/>
@@ -10189,7 +10189,7 @@
         <v>164</v>
       </c>
       <c r="Z45" s="163" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AA45" s="144">
         <f t="shared" si="1"/>
@@ -10202,7 +10202,7 @@
         <v>35</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D46" s="116"/>
       <c r="E46" s="116"/>
@@ -10267,7 +10267,7 @@
         <v>164</v>
       </c>
       <c r="Z46" s="163" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AA46" s="144">
         <f t="shared" si="1"/>
@@ -10280,7 +10280,7 @@
         <v>36</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D47" s="116"/>
       <c r="E47" s="116"/>
@@ -10345,7 +10345,7 @@
         <v>164</v>
       </c>
       <c r="Z47" s="163" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AA47" s="144">
         <f t="shared" si="1"/>
@@ -10358,7 +10358,7 @@
         <v>37</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D48" s="116"/>
       <c r="E48" s="116"/>
@@ -10423,7 +10423,7 @@
         <v>164</v>
       </c>
       <c r="Z48" s="163" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AA48" s="144">
         <f t="shared" si="1"/>
@@ -10436,7 +10436,7 @@
         <v>120</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D49" s="116"/>
       <c r="E49" s="116"/>
@@ -10501,7 +10501,7 @@
         <v>164</v>
       </c>
       <c r="Z49" s="163" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AA49" s="144">
         <f t="shared" si="1"/>
@@ -10514,7 +10514,7 @@
         <v>38</v>
       </c>
       <c r="C50" s="153" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D50" s="129"/>
       <c r="E50" s="129"/>
@@ -10594,7 +10594,7 @@
         <v>40</v>
       </c>
       <c r="C51" s="134" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D51" s="117"/>
       <c r="E51" s="117"/>
@@ -10659,7 +10659,7 @@
         <v>164</v>
       </c>
       <c r="Z51" s="162" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA51" s="143">
         <f t="shared" si="1"/>
@@ -10672,7 +10672,7 @@
         <v>41</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D52" s="116"/>
       <c r="E52" s="116"/>
@@ -10737,7 +10737,7 @@
         <v>164</v>
       </c>
       <c r="Z52" s="163" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA52" s="144">
         <f t="shared" si="1"/>
@@ -10750,7 +10750,7 @@
         <v>42</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D53" s="116"/>
       <c r="E53" s="116"/>
@@ -10815,7 +10815,7 @@
         <v>164</v>
       </c>
       <c r="Z53" s="163" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA53" s="144">
         <f t="shared" si="1"/>
@@ -10828,7 +10828,7 @@
         <v>43</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D54" s="116"/>
       <c r="E54" s="116"/>
@@ -10893,7 +10893,7 @@
         <v>164</v>
       </c>
       <c r="Z54" s="163" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA54" s="144">
         <f t="shared" si="1"/>
@@ -10906,7 +10906,7 @@
         <v>44</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D55" s="116"/>
       <c r="E55" s="116"/>
@@ -10971,7 +10971,7 @@
         <v>164</v>
       </c>
       <c r="Z55" s="163" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA55" s="144">
         <f t="shared" si="1"/>
@@ -10984,7 +10984,7 @@
         <v>45</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D56" s="116"/>
       <c r="E56" s="116"/>
@@ -11049,7 +11049,7 @@
         <v>164</v>
       </c>
       <c r="Z56" s="163" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA56" s="144">
         <f t="shared" si="1"/>
@@ -11062,7 +11062,7 @@
         <v>46</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D57" s="116"/>
       <c r="E57" s="116"/>
@@ -11127,7 +11127,7 @@
         <v>164</v>
       </c>
       <c r="Z57" s="163" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA57" s="144">
         <f t="shared" si="1"/>
@@ -11140,7 +11140,7 @@
         <v>47</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D58" s="116"/>
       <c r="E58" s="116"/>
@@ -11205,7 +11205,7 @@
         <v>164</v>
       </c>
       <c r="Z58" s="163" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA58" s="144">
         <f t="shared" si="1"/>
@@ -11218,7 +11218,7 @@
         <v>48</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D59" s="116"/>
       <c r="E59" s="116"/>
@@ -11283,7 +11283,7 @@
         <v>164</v>
       </c>
       <c r="Z59" s="163" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AA59" s="144">
         <f t="shared" si="1"/>
@@ -11296,7 +11296,7 @@
         <v>49</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D60" s="116"/>
       <c r="E60" s="116"/>
@@ -11357,7 +11357,7 @@
         <v>164</v>
       </c>
       <c r="Z60" s="163" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AA60" s="144">
         <f t="shared" si="1"/>
@@ -11370,7 +11370,7 @@
         <v>50</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D61" s="116"/>
       <c r="E61" s="116"/>
@@ -11431,7 +11431,7 @@
         <v>164</v>
       </c>
       <c r="Z61" s="163" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AA61" s="144">
         <f t="shared" si="1"/>
@@ -11444,7 +11444,7 @@
         <v>51</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D62" s="116"/>
       <c r="E62" s="116"/>
@@ -11509,7 +11509,7 @@
         <v>164</v>
       </c>
       <c r="Z62" s="163" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AA62" s="144">
         <f t="shared" si="1"/>
@@ -11522,7 +11522,7 @@
         <v>52</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D63" s="116"/>
       <c r="E63" s="116"/>
@@ -11587,7 +11587,7 @@
         <v>164</v>
       </c>
       <c r="Z63" s="163" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AA63" s="144">
         <f t="shared" si="1"/>
@@ -11600,7 +11600,7 @@
         <v>53</v>
       </c>
       <c r="C64" s="153" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D64" s="129"/>
       <c r="E64" s="129"/>
@@ -11665,7 +11665,7 @@
         <v>164</v>
       </c>
       <c r="Z64" s="152" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AA64" s="145">
         <f t="shared" si="1"/>
@@ -11680,7 +11680,7 @@
         <v>55</v>
       </c>
       <c r="C65" s="134" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D65" s="117"/>
       <c r="E65" s="117"/>
@@ -11745,7 +11745,7 @@
         <v>164</v>
       </c>
       <c r="Z65" s="184" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AA65" s="176">
         <f>COUNTIF(G65:Y65,"X")</f>
@@ -11758,7 +11758,7 @@
         <v>56</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D66" s="116"/>
       <c r="E66" s="116"/>
@@ -11823,7 +11823,7 @@
         <v>164</v>
       </c>
       <c r="Z66" s="163" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AA66" s="144">
         <f>COUNTIF(F66:Y66,"X")</f>
@@ -11836,7 +11836,7 @@
         <v>57</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D67" s="116"/>
       <c r="E67" s="116"/>
@@ -11901,7 +11901,7 @@
         <v>164</v>
       </c>
       <c r="Z67" s="163" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AA67" s="144">
         <f>COUNTIF(F67:Y67,"X")</f>
@@ -11914,7 +11914,7 @@
         <v>58</v>
       </c>
       <c r="C68" s="137" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D68" s="118"/>
       <c r="E68" s="118"/>
@@ -11979,7 +11979,7 @@
         <v>164</v>
       </c>
       <c r="Z68" s="152" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA68" s="145">
         <f>COUNTIF(F68:Y68,"X")</f>
@@ -12060,7 +12060,7 @@
       </c>
       <c r="W69" s="179">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="X69" s="179">
         <f t="shared" si="2"/>
@@ -12072,11 +12072,11 @@
       </c>
       <c r="Z69" s="177">
         <f>SUM(F69:Y69)</f>
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AA69" s="177">
         <f>SUM(AA3:AA68)</f>
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.25">
@@ -16067,7 +16067,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="121" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B1" s="197" t="s">
         <v>185</v>
@@ -16079,7 +16079,7 @@
         <v>149</v>
       </c>
       <c r="E1" s="198" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F1" s="198" t="s">
         <v>61</v>
@@ -16111,22 +16111,22 @@
         <v>150</v>
       </c>
       <c r="B2" s="134" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C2" s="204" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D2" s="204" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E2" s="134" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F2" s="134">
         <v>2015</v>
       </c>
       <c r="G2" s="187" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H2" s="205"/>
     </row>
@@ -16135,13 +16135,13 @@
         <v>169</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C3" s="200" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D3" s="200" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11">
@@ -16155,13 +16155,13 @@
         <v>151</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C4" s="200" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D4" s="200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11">
@@ -16175,13 +16175,13 @@
         <v>152</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C5" s="200" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D5" s="200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11">
@@ -16195,13 +16195,13 @@
         <v>168</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C6" s="200" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D6" s="200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11">
@@ -16215,22 +16215,22 @@
         <v>166</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C7" s="200" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D7" s="200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F7" s="11">
         <v>2015</v>
       </c>
       <c r="G7" s="212" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H7" s="207"/>
     </row>
@@ -16242,10 +16242,10 @@
         <v>189</v>
       </c>
       <c r="C8" s="200" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D8" s="200" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>191</v>
@@ -16263,13 +16263,13 @@
         <v>154</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C9" s="200" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D9" s="200" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="1">
@@ -16283,13 +16283,13 @@
         <v>175</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C10" s="200" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D10" s="200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="1">
@@ -16303,13 +16303,13 @@
         <v>155</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C11" s="200" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D11" s="200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="1">
@@ -16323,13 +16323,13 @@
         <v>156</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C12" s="200" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D12" s="200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E12" s="153"/>
       <c r="F12" s="1">
@@ -16343,22 +16343,22 @@
         <v>157</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C13" s="200" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D13" s="200" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F13" s="1">
         <v>2015</v>
       </c>
       <c r="G13" s="212" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H13" s="207"/>
     </row>
@@ -16370,10 +16370,10 @@
         <v>190</v>
       </c>
       <c r="C14" s="200" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D14" s="200" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>192</v>
@@ -16391,22 +16391,22 @@
         <v>165</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C15" s="200" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D15" s="200" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F15" s="11">
         <v>2015</v>
       </c>
       <c r="G15" s="212" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H15" s="207"/>
     </row>
@@ -16415,13 +16415,13 @@
         <v>159</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C16" s="200" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D16" s="200" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="1">
@@ -16435,22 +16435,22 @@
         <v>160</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C17" s="200" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D17" s="200" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F17" s="1">
         <v>2015</v>
       </c>
       <c r="G17" s="150" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H17" s="207"/>
     </row>
@@ -16459,22 +16459,22 @@
         <v>161</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C18" s="200" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D18" s="200" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F18" s="1">
         <v>2015</v>
       </c>
       <c r="G18" s="150" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H18" s="207"/>
     </row>
@@ -16483,16 +16483,16 @@
         <v>178</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C19" s="200" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D19" s="200" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E19" s="153" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F19" s="11">
         <v>2015</v>
@@ -16505,13 +16505,13 @@
         <v>182</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C20" s="200" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D20" s="200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="1">
@@ -16525,13 +16525,13 @@
         <v>162</v>
       </c>
       <c r="B21" s="137" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C21" s="209" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D21" s="209" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E21" s="137"/>
       <c r="F21" s="210">
@@ -16543,7 +16543,7 @@
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="273" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B26" s="274"/>
       <c r="C26" s="275"/>
@@ -16551,7 +16551,7 @@
     </row>
     <row r="27" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="272" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B27" s="272"/>
       <c r="C27" s="272"/>

</xml_diff>

<commit_message>
Updated energy, industry, residential temporal profile
</commit_message>
<xml_diff>
--- a/Datasets_summary.xlsx
+++ b/Datasets_summary.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R_projects\Spatialization\"/>
@@ -16,7 +16,7 @@
     <sheet name="Temporal distrib. - methodology" sheetId="2" r:id="rId2"/>
     <sheet name="Temporal distribution - summary" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1030,7 +1030,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6681,10 +6681,10 @@
   <dimension ref="A1:AA239"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Temporal profiles updated and finished
</commit_message>
<xml_diff>
--- a/Datasets_summary.xlsx
+++ b/Datasets_summary.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="296">
   <si>
     <t>NFR category</t>
   </si>
@@ -570,37 +570,19 @@
     <t>http://www.eps.rs/lat/kolubara/Stranice/Proizvodnja/Prerada.aspx</t>
   </si>
   <si>
-    <t>HE = WDWW + WT0024 + WT0624 + !PH + k*SA + k*HS + TEMP + !RP</t>
-  </si>
-  <si>
     <t>HE = WDWW + WT0816 + WT1624 + !PH + !RP</t>
   </si>
   <si>
     <t>COUNT</t>
   </si>
   <si>
-    <t>HE = WDWW + WT0024 + !PH + SA + !RP</t>
-  </si>
-  <si>
     <t>Working Weekends (WW)</t>
   </si>
   <si>
-    <t>HE = WDWW +DL + !PH + SA + SAAG</t>
-  </si>
-  <si>
     <t>HE = WD + WT0816 + WT1624 + WW + !PH + !RP</t>
   </si>
   <si>
     <t>Vehicles trend  activity (VA)</t>
-  </si>
-  <si>
-    <t>HE = WD + WT0816 + WT1624 + WW + RH0709 + RH1517 + !PH + VA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HE = WD + WT0816 + WT1624 + WE + RH0709 + RH1517 + !PH + TEMP + VA </t>
-  </si>
-  <si>
-    <t>HE = WD + WT0816 + DL + WE +  !PH + SA</t>
   </si>
   <si>
     <t>Number of flights per hour (NFH)</t>
@@ -647,32 +629,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Data collected from public service </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>dateandtime.com,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for 2015 year. Function was created from the data that describes season periods for the whole year.</t>
-    </r>
-  </si>
-  <si>
     <t>Sunrise, Sunset, and Daylength for Serbia in 2015 year</t>
   </si>
   <si>
@@ -733,9 +689,6 @@
     <t>The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed  by assuming that the domesting flights happen exclusively by day light and with the less activity in the winter.</t>
   </si>
   <si>
-    <t>HE = DL + SA</t>
-  </si>
-  <si>
     <t>The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed  by using the hourly counted vehice activity (on the 350 vehicle activity counters). The average hourly vehicle activity for the IA category will be used fo highway inventory. For the rural inventory, the average hourly vehicle activity for IIA and IB will be used. For the urban inventory, the activity graph will be constructed by assuming that the urban road activity is higher by day light, for the working days, for the rush hours as well as for the  public holidays.</t>
   </si>
   <si>
@@ -743,9 +696,6 @@
   </si>
   <si>
     <t>The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed  by assuming that the railway transport happens mostly during the day (day light). But with less activity during the public holidays, but with the increasing activity during the summer season.</t>
-  </si>
-  <si>
-    <t>HE = WDWW + DL  + WE + !PH + SA</t>
   </si>
   <si>
     <t>The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed  by assuming that the  "Commercial/institutional: Stationary Combustion" happens during the heating season with the increasing activity during the extreme winter, public holidays and less activity at night.</t>
@@ -967,9 +917,6 @@
     <t>HE = WDWW + (k+DL) + !PH + (k+SAAG) + inverse(TEMP) + SLP</t>
   </si>
   <si>
-    <t>HE = (k+DL) + (k+SA) + inverse(TEMP) + SLP</t>
-  </si>
-  <si>
     <t>HE = WDWW + (k+DL) + (k+SAAG) + inverse(TEMP) + SLP</t>
   </si>
   <si>
@@ -991,12 +938,6 @@
     <t>Working time for heating season [06-22h] (WT0622)</t>
   </si>
   <si>
-    <t>HE = WDWW + WT0024 + !PH + (k1*SA + k2) + !RP</t>
-  </si>
-  <si>
-    <t>HE = WDWW + WT0816 + WT1624 + !PH + (k1*SA + k2)</t>
-  </si>
-  <si>
     <t>HE = WDWW + DL + inverse(TEMP) + SLP + !PH</t>
   </si>
   <si>
@@ -1021,10 +962,77 @@
     <t xml:space="preserve">HE = WD + WT0816 + WT1624 + !PH </t>
   </si>
   <si>
-    <t>HE = WDWW + WT0816 + WT1624 + WE + !PH + SA</t>
-  </si>
-  <si>
     <t>The inventory emission from this sub - category will be temoral dissagregated based on identifed indicators  and equation. The temporal activity graph will be constructed  by assuming that the shipping transport happens mostly during the day (day light). But with less activity during the public holidays, weekends and winter season.</t>
+  </si>
+  <si>
+    <t>HE = WDWW +DL + !PH + TEMP + SAAG</t>
+  </si>
+  <si>
+    <t>HE = WDWW + WT0024 + WT0624 + !PH + k*HS + TEMP + !RP</t>
+  </si>
+  <si>
+    <t>HE = WDWW + WT0024 + !PH + TEMP + !RP</t>
+  </si>
+  <si>
+    <t>HE = (k+DL) + inverse(TEMP) + SLP</t>
+  </si>
+  <si>
+    <t>HE = WDWW + WT0816 + WT1624 + !PH + TEMP</t>
+  </si>
+  <si>
+    <t>HE = WD + WT0816 + WT1624 + WW + !PH + VA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HE = WD + WT0816 + WT1624 + WE + !PH + TEMP + VA </t>
+  </si>
+  <si>
+    <t>HE = WD + WT0816 + DL + WE +  !PH + TEMP</t>
+  </si>
+  <si>
+    <t>HE = DL + TEMP</t>
+  </si>
+  <si>
+    <t>HE = WDWW + WT0816 + WT1624 + WE + !PH + TEMP</t>
+  </si>
+  <si>
+    <t>HE = WDWW + DL  + WE + !PH + TEMP</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Data collected from public service </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dateandtime.com,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for 2015 year. Function was created from the data that describes season periods for the whole year.                                                                                      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>REPLACED with temperature, because it describes seasonality much better.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -4233,8 +4241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6680,11 +6688,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA239"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
+      <selection pane="bottomRight" activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6715,7 +6723,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="245" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="G1" s="246"/>
       <c r="H1" s="246"/>
@@ -6748,7 +6756,7 @@
         <v>148</v>
       </c>
       <c r="D2" s="110" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="E2" s="111" t="s">
         <v>115</v>
@@ -6769,7 +6777,7 @@
         <v>168</v>
       </c>
       <c r="K2" s="113" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="L2" s="113" t="s">
         <v>153</v>
@@ -6778,7 +6786,7 @@
         <v>154</v>
       </c>
       <c r="N2" s="113" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="O2" s="113" t="s">
         <v>155</v>
@@ -6805,10 +6813,10 @@
         <v>161</v>
       </c>
       <c r="W2" s="161" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="X2" s="161" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="Y2" s="114" t="s">
         <v>162</v>
@@ -6828,13 +6836,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="134" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D3" s="134" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E3" s="187" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F3" s="135" t="s">
         <v>164</v>
@@ -6873,7 +6881,7 @@
         <v>138</v>
       </c>
       <c r="R3" s="135" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="S3" s="135" t="s">
         <v>138</v>
@@ -6897,11 +6905,11 @@
         <v>138</v>
       </c>
       <c r="Z3" s="146" t="s">
-        <v>171</v>
+        <v>285</v>
       </c>
       <c r="AA3" s="124">
-        <f t="shared" ref="AA3:AA34" si="0">COUNTIF(F3:Y3,"X")</f>
-        <v>8</v>
+        <f>COUNTIF(F3:Y3,"X")</f>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -6910,10 +6918,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E4" s="116"/>
       <c r="F4" s="123" t="s">
@@ -6977,10 +6985,10 @@
         <v>138</v>
       </c>
       <c r="Z4" s="147" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="AA4" s="122">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F4:Y4,"X")</f>
         <v>3</v>
       </c>
     </row>
@@ -6990,7 +6998,7 @@
         <v>68</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D5" s="194"/>
       <c r="E5" s="116"/>
@@ -7055,10 +7063,10 @@
         <v>138</v>
       </c>
       <c r="Z5" s="147" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="AA5" s="122">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F5:Y5,"X")</f>
         <v>3</v>
       </c>
     </row>
@@ -7068,7 +7076,7 @@
         <v>69</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D6" s="194"/>
       <c r="E6" s="116"/>
@@ -7133,10 +7141,10 @@
         <v>138</v>
       </c>
       <c r="Z6" s="147" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="AA6" s="122">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F6:Y6,"X")</f>
         <v>3</v>
       </c>
     </row>
@@ -7146,7 +7154,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D7" s="194"/>
       <c r="E7" s="150" t="s">
@@ -7213,10 +7221,10 @@
         <v>138</v>
       </c>
       <c r="Z7" s="147" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AA7" s="122">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F7:Y7,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -7226,7 +7234,7 @@
         <v>70</v>
       </c>
       <c r="C8" s="153" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D8" s="195"/>
       <c r="E8" s="165" t="s">
@@ -7293,10 +7301,10 @@
         <v>138</v>
       </c>
       <c r="Z8" s="148" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AA8" s="128">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F8:Y8,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -7308,7 +7316,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="134" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D9" s="196"/>
       <c r="E9" s="117"/>
@@ -7349,7 +7357,7 @@
         <v>138</v>
       </c>
       <c r="R9" s="135" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="S9" s="135" t="s">
         <v>164</v>
@@ -7358,7 +7366,7 @@
         <v>164</v>
       </c>
       <c r="U9" s="135" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="V9" s="135" t="s">
         <v>164</v>
@@ -7373,10 +7381,10 @@
         <v>138</v>
       </c>
       <c r="Z9" s="162" t="s">
-        <v>174</v>
+        <v>286</v>
       </c>
       <c r="AA9" s="143">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F9:Y9,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -7386,7 +7394,7 @@
         <v>75</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D10" s="194"/>
       <c r="E10" s="116"/>
@@ -7451,10 +7459,10 @@
         <v>164</v>
       </c>
       <c r="Z10" s="163" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="AA10" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F10:Y10,"X")</f>
         <v>4</v>
       </c>
     </row>
@@ -7464,7 +7472,7 @@
         <v>111</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="D11" s="194"/>
       <c r="E11" s="116"/>
@@ -7529,10 +7537,10 @@
         <v>164</v>
       </c>
       <c r="Z11" s="163" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="AA11" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F11:Y11,"X")</f>
         <v>3</v>
       </c>
     </row>
@@ -7542,7 +7550,7 @@
         <v>76</v>
       </c>
       <c r="C12" s="153" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D12" s="195"/>
       <c r="E12" s="129"/>
@@ -7550,7 +7558,7 @@
         <v>164</v>
       </c>
       <c r="G12" s="130" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="H12" s="130" t="s">
         <v>164</v>
@@ -7559,7 +7567,7 @@
         <v>164</v>
       </c>
       <c r="J12" s="130" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="K12" s="130" t="s">
         <v>164</v>
@@ -7607,10 +7615,10 @@
         <v>164</v>
       </c>
       <c r="Z12" s="166" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="AA12" s="160">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F12:Y12,"X")</f>
         <v>3</v>
       </c>
     </row>
@@ -7622,7 +7630,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="134" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="D13" s="134"/>
       <c r="E13" s="117"/>
@@ -7687,10 +7695,10 @@
         <v>164</v>
       </c>
       <c r="Z13" s="140" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="AA13" s="143">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F13:Y13,"X")</f>
         <v>1</v>
       </c>
     </row>
@@ -7700,7 +7708,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D14" s="194"/>
       <c r="E14" s="116"/>
@@ -7741,7 +7749,7 @@
         <v>164</v>
       </c>
       <c r="R14" s="123" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="S14" s="123" t="s">
         <v>164</v>
@@ -7750,7 +7758,7 @@
         <v>164</v>
       </c>
       <c r="U14" s="123" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="V14" s="123" t="s">
         <v>164</v>
@@ -7765,10 +7773,10 @@
         <v>164</v>
       </c>
       <c r="Z14" s="141" t="s">
-        <v>210</v>
+        <v>292</v>
       </c>
       <c r="AA14" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F14:Y14,"X")</f>
         <v>2</v>
       </c>
     </row>
@@ -7778,7 +7786,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D15" s="194"/>
       <c r="E15" s="116"/>
@@ -7843,10 +7851,10 @@
         <v>164</v>
       </c>
       <c r="Z15" s="141" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AA15" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F15:Y15,"X")</f>
         <v>10</v>
       </c>
     </row>
@@ -7856,7 +7864,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D16" s="194"/>
       <c r="E16" s="116"/>
@@ -7921,10 +7929,10 @@
         <v>164</v>
       </c>
       <c r="Z16" s="141" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AA16" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F16:Y16,"X")</f>
         <v>10</v>
       </c>
     </row>
@@ -7934,7 +7942,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D17" s="194"/>
       <c r="E17" s="116"/>
@@ -7999,10 +8007,10 @@
         <v>164</v>
       </c>
       <c r="Z17" s="141" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AA17" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F17:Y17,"X")</f>
         <v>10</v>
       </c>
     </row>
@@ -8012,7 +8020,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D18" s="194"/>
       <c r="E18" s="116"/>
@@ -8077,10 +8085,10 @@
         <v>164</v>
       </c>
       <c r="Z18" s="141" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AA18" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F18:Y18,"X")</f>
         <v>10</v>
       </c>
     </row>
@@ -8090,7 +8098,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D19" s="194"/>
       <c r="E19" s="116"/>
@@ -8155,10 +8163,10 @@
         <v>164</v>
       </c>
       <c r="Z19" s="141" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AA19" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F19:Y19,"X")</f>
         <v>10</v>
       </c>
     </row>
@@ -8168,7 +8176,7 @@
         <v>15</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D20" s="194"/>
       <c r="E20" s="116"/>
@@ -8233,10 +8241,10 @@
         <v>164</v>
       </c>
       <c r="Z20" s="141" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AA20" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F20:Y20,"X")</f>
         <v>10</v>
       </c>
     </row>
@@ -8246,7 +8254,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D21" s="194"/>
       <c r="E21" s="116"/>
@@ -8311,10 +8319,10 @@
         <v>164</v>
       </c>
       <c r="Z21" s="141" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AA21" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F21:Y21,"X")</f>
         <v>10</v>
       </c>
     </row>
@@ -8324,7 +8332,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D22" s="194"/>
       <c r="E22" s="116"/>
@@ -8389,10 +8397,10 @@
         <v>164</v>
       </c>
       <c r="Z22" s="141" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="AA22" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F22:Y22,"X")</f>
         <v>10</v>
       </c>
     </row>
@@ -8402,7 +8410,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D23" s="194"/>
       <c r="E23" s="116"/>
@@ -8443,7 +8451,7 @@
         <v>138</v>
       </c>
       <c r="R23" s="123" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="S23" s="123" t="s">
         <v>164</v>
@@ -8452,7 +8460,7 @@
         <v>164</v>
       </c>
       <c r="U23" s="123" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="V23" s="123" t="s">
         <v>164</v>
@@ -8467,10 +8475,10 @@
         <v>164</v>
       </c>
       <c r="Z23" s="141" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="AA23" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F23:Y23,"X")</f>
         <v>6</v>
       </c>
     </row>
@@ -8480,7 +8488,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="153" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="D24" s="195"/>
       <c r="E24" s="129"/>
@@ -8521,7 +8529,7 @@
         <v>138</v>
       </c>
       <c r="R24" s="130" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="S24" s="130" t="s">
         <v>164</v>
@@ -8530,7 +8538,7 @@
         <v>164</v>
       </c>
       <c r="U24" s="130" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="V24" s="130" t="s">
         <v>164</v>
@@ -8545,10 +8553,10 @@
         <v>164</v>
       </c>
       <c r="Z24" s="142" t="s">
-        <v>214</v>
+        <v>294</v>
       </c>
       <c r="AA24" s="145">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F24:Y24,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -8560,7 +8568,7 @@
         <v>91</v>
       </c>
       <c r="C25" s="134" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D25" s="196"/>
       <c r="E25" s="117"/>
@@ -8625,10 +8633,10 @@
         <v>164</v>
       </c>
       <c r="Z25" s="184" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="AA25" s="176">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F25:Y25,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -8638,7 +8646,7 @@
         <v>93</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="D26" s="194"/>
       <c r="E26" s="116"/>
@@ -8703,10 +8711,10 @@
         <v>164</v>
       </c>
       <c r="Z26" s="163" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="AA26" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F26:Y26,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -8716,7 +8724,7 @@
         <v>92</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="D27" s="194"/>
       <c r="E27" s="116"/>
@@ -8757,7 +8765,7 @@
         <v>138</v>
       </c>
       <c r="R27" s="123" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="S27" s="123" t="s">
         <v>164</v>
@@ -8766,7 +8774,7 @@
         <v>138</v>
       </c>
       <c r="U27" s="123" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="V27" s="123" t="s">
         <v>164</v>
@@ -8781,10 +8789,10 @@
         <v>164</v>
       </c>
       <c r="Z27" s="163" t="s">
-        <v>176</v>
+        <v>284</v>
       </c>
       <c r="AA27" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F27:Y27,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -8794,7 +8802,7 @@
         <v>21</v>
       </c>
       <c r="C28" s="153" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D28" s="195"/>
       <c r="E28" s="129"/>
@@ -8835,7 +8843,7 @@
         <v>138</v>
       </c>
       <c r="R28" s="130" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="S28" s="130" t="s">
         <v>164</v>
@@ -8843,8 +8851,8 @@
       <c r="T28" s="130" t="s">
         <v>138</v>
       </c>
-      <c r="U28" s="130" t="s">
-        <v>164</v>
+      <c r="U28" s="123" t="s">
+        <v>138</v>
       </c>
       <c r="V28" s="130" t="s">
         <v>164</v>
@@ -8859,10 +8867,10 @@
         <v>164</v>
       </c>
       <c r="Z28" s="166" t="s">
-        <v>176</v>
+        <v>284</v>
       </c>
       <c r="AA28" s="160">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F28:Y28,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -8874,7 +8882,7 @@
         <v>23</v>
       </c>
       <c r="C29" s="134" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D29" s="117"/>
       <c r="E29" s="117"/>
@@ -8939,10 +8947,10 @@
         <v>138</v>
       </c>
       <c r="Z29" s="162" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AA29" s="143">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F29:Y29,"X")</f>
         <v>6</v>
       </c>
     </row>
@@ -8952,7 +8960,7 @@
         <v>104</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D30" s="116"/>
       <c r="E30" s="116"/>
@@ -9017,10 +9025,10 @@
         <v>138</v>
       </c>
       <c r="Z30" s="163" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AA30" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F30:Y30,"X")</f>
         <v>6</v>
       </c>
     </row>
@@ -9030,7 +9038,7 @@
         <v>106</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D31" s="116"/>
       <c r="E31" s="116"/>
@@ -9095,10 +9103,10 @@
         <v>138</v>
       </c>
       <c r="Z31" s="163" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AA31" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F31:Y31,"X")</f>
         <v>6</v>
       </c>
     </row>
@@ -9108,7 +9116,7 @@
         <v>105</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D32" s="116"/>
       <c r="E32" s="116"/>
@@ -9173,10 +9181,10 @@
         <v>138</v>
       </c>
       <c r="Z32" s="163" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AA32" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F32:Y32,"X")</f>
         <v>6</v>
       </c>
     </row>
@@ -9186,7 +9194,7 @@
         <v>107</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D33" s="116"/>
       <c r="E33" s="116"/>
@@ -9251,10 +9259,10 @@
         <v>138</v>
       </c>
       <c r="Z33" s="163" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AA33" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F33:Y33,"X")</f>
         <v>6</v>
       </c>
     </row>
@@ -9264,7 +9272,7 @@
         <v>109</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D34" s="116"/>
       <c r="E34" s="116"/>
@@ -9329,10 +9337,10 @@
         <v>138</v>
       </c>
       <c r="Z34" s="163" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AA34" s="144">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(F34:Y34,"X")</f>
         <v>6</v>
       </c>
     </row>
@@ -9342,7 +9350,7 @@
         <v>24</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D35" s="116"/>
       <c r="E35" s="116"/>
@@ -9407,10 +9415,10 @@
         <v>138</v>
       </c>
       <c r="Z35" s="163" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AA35" s="144">
-        <f t="shared" ref="AA35:AA64" si="1">COUNTIF(F35:Y35,"X")</f>
+        <f>COUNTIF(F35:Y35,"X")</f>
         <v>6</v>
       </c>
     </row>
@@ -9420,7 +9428,7 @@
         <v>25</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D36" s="116"/>
       <c r="E36" s="116"/>
@@ -9485,10 +9493,10 @@
         <v>138</v>
       </c>
       <c r="Z36" s="163" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AA36" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F36:Y36,"X")</f>
         <v>6</v>
       </c>
     </row>
@@ -9498,7 +9506,7 @@
         <v>26</v>
       </c>
       <c r="C37" s="137" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D37" s="118"/>
       <c r="E37" s="118"/>
@@ -9563,10 +9571,10 @@
         <v>138</v>
       </c>
       <c r="Z37" s="166" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AA37" s="160">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F37:Y37,"X")</f>
         <v>6</v>
       </c>
     </row>
@@ -9578,7 +9586,7 @@
         <v>27</v>
       </c>
       <c r="C38" s="189" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D38" s="190"/>
       <c r="E38" s="190"/>
@@ -9619,7 +9627,7 @@
         <v>138</v>
       </c>
       <c r="R38" s="191" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="S38" s="191" t="s">
         <v>164</v>
@@ -9628,7 +9636,7 @@
         <v>164</v>
       </c>
       <c r="U38" s="191" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="V38" s="191" t="s">
         <v>164</v>
@@ -9643,10 +9651,10 @@
         <v>138</v>
       </c>
       <c r="Z38" s="162" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AA38" s="143">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F38:Y38,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -9656,7 +9664,7 @@
         <v>28</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D39" s="116"/>
       <c r="E39" s="116"/>
@@ -9697,7 +9705,7 @@
         <v>138</v>
       </c>
       <c r="R39" s="123" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="S39" s="123" t="s">
         <v>164</v>
@@ -9706,7 +9714,7 @@
         <v>164</v>
       </c>
       <c r="U39" s="123" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="V39" s="123" t="s">
         <v>164</v>
@@ -9721,10 +9729,10 @@
         <v>164</v>
       </c>
       <c r="Z39" s="163" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="AA39" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F39:Y39,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -9734,7 +9742,7 @@
         <v>29</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D40" s="116"/>
       <c r="E40" s="116"/>
@@ -9766,10 +9774,10 @@
         <v>138</v>
       </c>
       <c r="O40" s="123" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="P40" s="123" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="Q40" s="123" t="s">
         <v>138</v>
@@ -9799,11 +9807,11 @@
         <v>164</v>
       </c>
       <c r="Z40" s="163" t="s">
-        <v>179</v>
+        <v>289</v>
       </c>
       <c r="AA40" s="144">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f>COUNTIF(F40:Y40,"X")</f>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -9812,7 +9820,7 @@
         <v>30</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="D41" s="116"/>
       <c r="E41" s="116"/>
@@ -9877,10 +9885,10 @@
         <v>164</v>
       </c>
       <c r="Z41" s="163" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="AA41" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F41:Y41,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -9890,7 +9898,7 @@
         <v>31</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D42" s="116"/>
       <c r="E42" s="116"/>
@@ -9922,10 +9930,10 @@
         <v>164</v>
       </c>
       <c r="O42" s="123" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="P42" s="123" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="Q42" s="123" t="s">
         <v>138</v>
@@ -9955,11 +9963,11 @@
         <v>164</v>
       </c>
       <c r="Z42" s="163" t="s">
-        <v>180</v>
+        <v>290</v>
       </c>
       <c r="AA42" s="144">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f>COUNTIF(F42:Y42,"X")</f>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -9968,7 +9976,7 @@
         <v>32</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D43" s="116"/>
       <c r="E43" s="116"/>
@@ -10000,10 +10008,10 @@
         <v>164</v>
       </c>
       <c r="O43" s="123" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="P43" s="123" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="Q43" s="123" t="s">
         <v>138</v>
@@ -10033,11 +10041,11 @@
         <v>164</v>
       </c>
       <c r="Z43" s="163" t="s">
-        <v>180</v>
+        <v>290</v>
       </c>
       <c r="AA43" s="144">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f>COUNTIF(F43:Y43,"X")</f>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -10046,7 +10054,7 @@
         <v>33</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D44" s="116"/>
       <c r="E44" s="116"/>
@@ -10078,10 +10086,10 @@
         <v>164</v>
       </c>
       <c r="O44" s="123" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="P44" s="123" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="Q44" s="123" t="s">
         <v>138</v>
@@ -10111,11 +10119,11 @@
         <v>164</v>
       </c>
       <c r="Z44" s="163" t="s">
-        <v>180</v>
+        <v>290</v>
       </c>
       <c r="AA44" s="144">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f>COUNTIF(F44:Y44,"X")</f>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -10124,7 +10132,7 @@
         <v>34</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="D45" s="116"/>
       <c r="E45" s="116"/>
@@ -10189,10 +10197,10 @@
         <v>164</v>
       </c>
       <c r="Z45" s="163" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="AA45" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F45:Y45,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -10202,7 +10210,7 @@
         <v>35</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="D46" s="116"/>
       <c r="E46" s="116"/>
@@ -10267,10 +10275,10 @@
         <v>164</v>
       </c>
       <c r="Z46" s="163" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="AA46" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F46:Y46,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -10280,7 +10288,7 @@
         <v>36</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="D47" s="116"/>
       <c r="E47" s="116"/>
@@ -10345,10 +10353,10 @@
         <v>164</v>
       </c>
       <c r="Z47" s="163" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="AA47" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F47:Y47,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -10358,7 +10366,7 @@
         <v>37</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="D48" s="116"/>
       <c r="E48" s="116"/>
@@ -10423,10 +10431,10 @@
         <v>164</v>
       </c>
       <c r="Z48" s="163" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="AA48" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F48:Y48,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -10436,7 +10444,7 @@
         <v>120</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="D49" s="116"/>
       <c r="E49" s="116"/>
@@ -10501,10 +10509,10 @@
         <v>164</v>
       </c>
       <c r="Z49" s="163" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="AA49" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F49:Y49,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -10514,7 +10522,7 @@
         <v>38</v>
       </c>
       <c r="C50" s="153" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D50" s="129"/>
       <c r="E50" s="129"/>
@@ -10555,7 +10563,7 @@
         <v>138</v>
       </c>
       <c r="R50" s="130" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="S50" s="130" t="s">
         <v>164</v>
@@ -10564,7 +10572,7 @@
         <v>164</v>
       </c>
       <c r="U50" s="130" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="V50" s="130" t="s">
         <v>164</v>
@@ -10579,10 +10587,10 @@
         <v>164</v>
       </c>
       <c r="Z50" s="166" t="s">
-        <v>181</v>
+        <v>291</v>
       </c>
       <c r="AA50" s="160">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F50:Y50,"X")</f>
         <v>6</v>
       </c>
     </row>
@@ -10594,7 +10602,7 @@
         <v>40</v>
       </c>
       <c r="C51" s="134" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="D51" s="117"/>
       <c r="E51" s="117"/>
@@ -10659,10 +10667,10 @@
         <v>164</v>
       </c>
       <c r="Z51" s="162" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="AA51" s="143">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F51:Y51,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -10672,7 +10680,7 @@
         <v>41</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D52" s="116"/>
       <c r="E52" s="116"/>
@@ -10737,10 +10745,10 @@
         <v>164</v>
       </c>
       <c r="Z52" s="163" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="AA52" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F52:Y52,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -10750,7 +10758,7 @@
         <v>42</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D53" s="116"/>
       <c r="E53" s="116"/>
@@ -10815,10 +10823,10 @@
         <v>164</v>
       </c>
       <c r="Z53" s="163" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="AA53" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F53:Y53,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -10828,7 +10836,7 @@
         <v>43</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D54" s="116"/>
       <c r="E54" s="116"/>
@@ -10893,10 +10901,10 @@
         <v>164</v>
       </c>
       <c r="Z54" s="163" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="AA54" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F54:Y54,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -10906,7 +10914,7 @@
         <v>44</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D55" s="116"/>
       <c r="E55" s="116"/>
@@ -10971,10 +10979,10 @@
         <v>164</v>
       </c>
       <c r="Z55" s="163" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="AA55" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F55:Y55,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -10984,7 +10992,7 @@
         <v>45</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D56" s="116"/>
       <c r="E56" s="116"/>
@@ -11049,10 +11057,10 @@
         <v>164</v>
       </c>
       <c r="Z56" s="163" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="AA56" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F56:Y56,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -11062,7 +11070,7 @@
         <v>46</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D57" s="116"/>
       <c r="E57" s="116"/>
@@ -11127,10 +11135,10 @@
         <v>164</v>
       </c>
       <c r="Z57" s="163" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="AA57" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F57:Y57,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -11140,7 +11148,7 @@
         <v>47</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D58" s="116"/>
       <c r="E58" s="116"/>
@@ -11205,10 +11213,10 @@
         <v>164</v>
       </c>
       <c r="Z58" s="163" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="AA58" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F58:Y58,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -11218,7 +11226,7 @@
         <v>48</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D59" s="116"/>
       <c r="E59" s="116"/>
@@ -11283,10 +11291,10 @@
         <v>164</v>
       </c>
       <c r="Z59" s="163" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="AA59" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F59:Y59,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -11296,7 +11304,7 @@
         <v>49</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="D60" s="116"/>
       <c r="E60" s="116"/>
@@ -11357,10 +11365,10 @@
         <v>164</v>
       </c>
       <c r="Z60" s="163" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="AA60" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F60:Y60,"X")</f>
         <v>6</v>
       </c>
     </row>
@@ -11370,7 +11378,7 @@
         <v>50</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="D61" s="116"/>
       <c r="E61" s="116"/>
@@ -11431,10 +11439,10 @@
         <v>164</v>
       </c>
       <c r="Z61" s="163" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="AA61" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F61:Y61,"X")</f>
         <v>6</v>
       </c>
     </row>
@@ -11444,7 +11452,7 @@
         <v>51</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="D62" s="116"/>
       <c r="E62" s="116"/>
@@ -11485,7 +11493,7 @@
         <v>164</v>
       </c>
       <c r="R62" s="123" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="S62" s="123" t="s">
         <v>164</v>
@@ -11509,11 +11517,11 @@
         <v>164</v>
       </c>
       <c r="Z62" s="163" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="AA62" s="144">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f>COUNTIF(F62:Y62,"X")</f>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
@@ -11522,7 +11530,7 @@
         <v>52</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="D63" s="116"/>
       <c r="E63" s="116"/>
@@ -11587,10 +11595,10 @@
         <v>164</v>
       </c>
       <c r="Z63" s="163" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="AA63" s="144">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F63:Y63,"X")</f>
         <v>5</v>
       </c>
     </row>
@@ -11600,7 +11608,7 @@
         <v>53</v>
       </c>
       <c r="C64" s="153" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="D64" s="129"/>
       <c r="E64" s="129"/>
@@ -11665,10 +11673,10 @@
         <v>164</v>
       </c>
       <c r="Z64" s="152" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="AA64" s="145">
-        <f t="shared" si="1"/>
+        <f>COUNTIF(F64:Y64,"X")</f>
         <v>6</v>
       </c>
     </row>
@@ -11680,7 +11688,7 @@
         <v>55</v>
       </c>
       <c r="C65" s="134" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="D65" s="117"/>
       <c r="E65" s="117"/>
@@ -11745,7 +11753,7 @@
         <v>164</v>
       </c>
       <c r="Z65" s="184" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="AA65" s="176">
         <f>COUNTIF(G65:Y65,"X")</f>
@@ -11758,7 +11766,7 @@
         <v>56</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="D66" s="116"/>
       <c r="E66" s="116"/>
@@ -11823,7 +11831,7 @@
         <v>164</v>
       </c>
       <c r="Z66" s="163" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="AA66" s="144">
         <f>COUNTIF(F66:Y66,"X")</f>
@@ -11836,7 +11844,7 @@
         <v>57</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="D67" s="116"/>
       <c r="E67" s="116"/>
@@ -11901,7 +11909,7 @@
         <v>164</v>
       </c>
       <c r="Z67" s="163" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="AA67" s="144">
         <f>COUNTIF(F67:Y67,"X")</f>
@@ -11914,7 +11922,7 @@
         <v>58</v>
       </c>
       <c r="C68" s="137" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D68" s="118"/>
       <c r="E68" s="118"/>
@@ -11979,7 +11987,7 @@
         <v>164</v>
       </c>
       <c r="Z68" s="152" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="AA68" s="145">
         <f>COUNTIF(F68:Y68,"X")</f>
@@ -11988,95 +11996,95 @@
     </row>
     <row r="69" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E69" s="172" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F69" s="178">
         <f>COUNTIF(F3:F68,"X")</f>
         <v>25</v>
       </c>
       <c r="G69" s="179">
-        <f t="shared" ref="G69:Y69" si="2">COUNTIF(G3:G68,"X")</f>
+        <f t="shared" ref="G69:Y69" si="0">COUNTIF(G3:G68,"X")</f>
         <v>38</v>
       </c>
       <c r="H69" s="179">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="I69" s="179">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="J69" s="179">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="K69" s="179">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="L69" s="179">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="M69" s="179">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="N69" s="179">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="O69" s="179">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="P69" s="179">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="Q69" s="179">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="R69" s="179">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S69" s="179">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="T69" s="179">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="U69" s="179">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="V69" s="179">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="W69" s="179">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="P69" s="179">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="Q69" s="179">
-        <f t="shared" si="2"/>
-        <v>48</v>
-      </c>
-      <c r="R69" s="179">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="S69" s="179">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="T69" s="179">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="U69" s="179">
-        <f t="shared" si="2"/>
-        <v>36</v>
-      </c>
-      <c r="V69" s="179">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="W69" s="179">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
       <c r="X69" s="179">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Y69" s="180">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="Z69" s="177">
         <f>SUM(F69:Y69)</f>
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="AA69" s="177">
         <f>SUM(AA3:AA68)</f>
-        <v>377</v>
+        <v>367</v>
       </c>
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.25">
@@ -16050,8 +16058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16067,19 +16075,19 @@
   <sheetData>
     <row r="1" spans="1:23" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="121" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="B1" s="197" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C1" s="198" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D1" s="198" t="s">
         <v>149</v>
       </c>
       <c r="E1" s="198" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="F1" s="198" t="s">
         <v>61</v>
@@ -16088,7 +16096,7 @@
         <v>115</v>
       </c>
       <c r="H1" s="199" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="I1" s="186"/>
       <c r="J1" s="186"/>
@@ -16111,22 +16119,22 @@
         <v>150</v>
       </c>
       <c r="B2" s="134" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="C2" s="204" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="D2" s="204" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E2" s="134" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="F2" s="134">
         <v>2015</v>
       </c>
       <c r="G2" s="187" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="H2" s="205"/>
     </row>
@@ -16135,13 +16143,13 @@
         <v>169</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C3" s="200" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="D3" s="200" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11">
@@ -16155,13 +16163,13 @@
         <v>151</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C4" s="200" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D4" s="200" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11">
@@ -16175,13 +16183,13 @@
         <v>152</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" s="200" t="s">
+        <v>228</v>
+      </c>
+      <c r="D5" s="200" t="s">
         <v>244</v>
-      </c>
-      <c r="C5" s="200" t="s">
-        <v>237</v>
-      </c>
-      <c r="D5" s="200" t="s">
-        <v>253</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11">
@@ -16195,13 +16203,13 @@
         <v>168</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="C6" s="200" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D6" s="200" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11">
@@ -16215,22 +16223,22 @@
         <v>166</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C7" s="200" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D7" s="200" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="F7" s="11">
         <v>2015</v>
       </c>
       <c r="G7" s="212" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="H7" s="207"/>
     </row>
@@ -16239,22 +16247,22 @@
         <v>153</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C8" s="200" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D8" s="200" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="F8" s="11">
         <v>2015</v>
       </c>
       <c r="G8" s="150" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="H8" s="207"/>
     </row>
@@ -16263,13 +16271,13 @@
         <v>154</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="C9" s="200" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="D9" s="200" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="1">
@@ -16280,16 +16288,16 @@
     </row>
     <row r="10" spans="1:23" ht="408.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="206" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C10" s="200" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D10" s="200" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="1">
@@ -16303,13 +16311,13 @@
         <v>155</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C11" s="200" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D11" s="200" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="1">
@@ -16323,13 +16331,13 @@
         <v>156</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C12" s="200" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D12" s="200" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="E12" s="153"/>
       <c r="F12" s="1">
@@ -16343,22 +16351,22 @@
         <v>157</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C13" s="200" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="D13" s="200" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="F13" s="1">
         <v>2015</v>
       </c>
       <c r="G13" s="212" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="H13" s="207"/>
     </row>
@@ -16367,22 +16375,22 @@
         <v>158</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>189</v>
+        <v>295</v>
       </c>
       <c r="C14" s="200" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="D14" s="200" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="F14" s="11">
         <v>2015</v>
       </c>
       <c r="G14" s="150" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="H14" s="207"/>
     </row>
@@ -16391,22 +16399,22 @@
         <v>165</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C15" s="200" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="D15" s="200" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="F15" s="11">
         <v>2015</v>
       </c>
       <c r="G15" s="212" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="H15" s="207"/>
     </row>
@@ -16415,13 +16423,13 @@
         <v>159</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C16" s="200" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="D16" s="200" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="1">
@@ -16435,22 +16443,22 @@
         <v>160</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C17" s="200" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="D17" s="200" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="F17" s="1">
         <v>2015</v>
       </c>
       <c r="G17" s="150" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="H17" s="207"/>
     </row>
@@ -16459,40 +16467,40 @@
         <v>161</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C18" s="200" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="D18" s="200" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="F18" s="1">
         <v>2015</v>
       </c>
       <c r="G18" s="150" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="H18" s="207"/>
     </row>
     <row r="19" spans="1:8" ht="408.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="206" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C19" s="200" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="D19" s="200" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E19" s="153" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="F19" s="11">
         <v>2015</v>
@@ -16502,16 +16510,16 @@
     </row>
     <row r="20" spans="1:8" ht="408.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="206" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C20" s="200" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D20" s="200" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="1">
@@ -16525,13 +16533,13 @@
         <v>162</v>
       </c>
       <c r="B21" s="137" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C21" s="209" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="D21" s="209" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E21" s="137"/>
       <c r="F21" s="210">
@@ -16543,7 +16551,7 @@
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="273" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B26" s="274"/>
       <c r="C26" s="275"/>
@@ -16551,7 +16559,7 @@
     </row>
     <row r="27" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="272" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="B27" s="272"/>
       <c r="C27" s="272"/>

</xml_diff>

<commit_message>
Fugitive emissions spatialization updated
</commit_message>
<xml_diff>
--- a/Datasets_summary.xlsx
+++ b/Datasets_summary.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R_projects\Spatialization\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26595" windowHeight="11580"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Temporal distrib. - methodology" sheetId="2" r:id="rId2"/>
     <sheet name="Temporal distribution - summary" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2328" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2326" uniqueCount="337">
   <si>
     <t>NFR category</t>
   </si>
@@ -1238,11 +1243,17 @@
   <si>
     <t>The Total inventory was spatially allocated to the areas that represents the Solid waste disposal. For thus purpose, the dump sites will be extracted from the Corine Land Cover data (class 1.3.2 the of Corine Land Cover). Spatial allocation on 5x5km cells was conducted proportionally to the areas of the dump site that lies in each cell.</t>
   </si>
+  <si>
+    <t xml:space="preserve">Spatial Locations of rafineries are identified as sources from Energy category. </t>
+  </si>
+  <si>
+    <t>Spatial Locations of rafineries are identified as sources from Energy category.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1357,7 +1368,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1424,12 +1435,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="65">
     <border>
@@ -2884,6 +2889,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2953,102 +2961,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3056,12 +2968,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3073,60 +2979,159 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4519,7 +4524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4529,8 +4534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4541,7 +4546,7 @@
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="56.42578125" style="271" customWidth="1"/>
+    <col min="7" max="7" width="56.42578125" style="217" customWidth="1"/>
     <col min="8" max="8" width="49.28515625" customWidth="1"/>
     <col min="9" max="9" width="35.7109375" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" customWidth="1"/>
@@ -4555,11 +4560,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K1" s="222" t="s">
+      <c r="K1" s="223" t="s">
         <v>134</v>
       </c>
-      <c r="L1" s="223"/>
-      <c r="M1" s="224"/>
+      <c r="L1" s="224"/>
+      <c r="M1" s="225"/>
     </row>
     <row r="2" spans="1:16" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="46" t="s">
@@ -4612,7 +4617,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="238" t="s">
+      <c r="A3" s="239" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -4630,7 +4635,7 @@
       <c r="F3" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="272" t="s">
+      <c r="G3" s="241" t="s">
         <v>297</v>
       </c>
       <c r="H3" s="3"/>
@@ -4648,7 +4653,7 @@
       <c r="P3" s="59"/>
     </row>
     <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="239"/>
+      <c r="A4" s="240"/>
       <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
@@ -4664,7 +4669,7 @@
       <c r="F4" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="273"/>
+      <c r="G4" s="242"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -4680,7 +4685,7 @@
       <c r="P4" s="61"/>
     </row>
     <row r="5" spans="1:16" ht="36" x14ac:dyDescent="0.25">
-      <c r="A5" s="239"/>
+      <c r="A5" s="240"/>
       <c r="B5" s="9" t="s">
         <v>68</v>
       </c>
@@ -4696,7 +4701,7 @@
       <c r="F5" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="273"/>
+      <c r="G5" s="242"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -4712,7 +4717,7 @@
       <c r="P5" s="61"/>
     </row>
     <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="239"/>
+      <c r="A6" s="240"/>
       <c r="B6" s="9" t="s">
         <v>69</v>
       </c>
@@ -4728,7 +4733,7 @@
       <c r="F6" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="273"/>
+      <c r="G6" s="242"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -4744,7 +4749,7 @@
       <c r="P6" s="61"/>
     </row>
     <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="239"/>
+      <c r="A7" s="240"/>
       <c r="B7" s="9" t="s">
         <v>4</v>
       </c>
@@ -4760,7 +4765,7 @@
       <c r="F7" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="273"/>
+      <c r="G7" s="242"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -4776,7 +4781,7 @@
       <c r="P7" s="61"/>
     </row>
     <row r="8" spans="1:16" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="239"/>
+      <c r="A8" s="240"/>
       <c r="B8" s="9" t="s">
         <v>70</v>
       </c>
@@ -4792,7 +4797,7 @@
       <c r="F8" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="G8" s="274"/>
+      <c r="G8" s="243"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -4808,7 +4813,7 @@
       <c r="P8" s="63"/>
     </row>
     <row r="9" spans="1:16" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="227" t="s">
+      <c r="A9" s="228" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -4823,7 +4828,7 @@
       <c r="E9" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="280" t="s">
         <v>71</v>
       </c>
       <c r="G9" s="42" t="s">
@@ -4850,32 +4855,28 @@
       <c r="P9" s="59"/>
     </row>
     <row r="10" spans="1:16" s="290" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A10" s="228"/>
-      <c r="B10" s="280" t="s">
+      <c r="A10" s="229"/>
+      <c r="B10" s="13" t="s">
         <v>75</v>
       </c>
       <c r="C10" s="281" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="281" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E10" s="281" t="s">
         <v>67</v>
       </c>
       <c r="F10" s="281" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="282"/>
-      <c r="H10" s="283" t="s">
-        <v>77</v>
-      </c>
-      <c r="I10" s="283" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" s="284">
-        <v>2015</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="G10" s="282" t="s">
+        <v>335</v>
+      </c>
+      <c r="H10" s="283"/>
+      <c r="I10" s="283"/>
+      <c r="J10" s="284"/>
       <c r="K10" s="285" t="s">
         <v>138</v>
       </c>
@@ -4886,7 +4887,7 @@
       <c r="P10" s="289"/>
     </row>
     <row r="11" spans="1:16" ht="120" x14ac:dyDescent="0.25">
-      <c r="A11" s="228"/>
+      <c r="A11" s="229"/>
       <c r="B11" s="13" t="s">
         <v>111</v>
       </c>
@@ -4924,43 +4925,39 @@
       <c r="P11" s="61"/>
     </row>
     <row r="12" spans="1:16" s="290" customFormat="1" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="229"/>
-      <c r="B12" s="291" t="s">
+      <c r="A12" s="230"/>
+      <c r="B12" s="298" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="292" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="292" t="s">
+      <c r="C12" s="291" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="292" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="292" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="293"/>
-      <c r="H12" s="294" t="s">
-        <v>77</v>
-      </c>
-      <c r="I12" s="294" t="s">
-        <v>78</v>
-      </c>
-      <c r="J12" s="295">
-        <v>2015</v>
-      </c>
-      <c r="K12" s="296" t="s">
-        <v>138</v>
-      </c>
-      <c r="L12" s="297"/>
-      <c r="M12" s="297"/>
-      <c r="N12" s="298"/>
+      <c r="D12" s="291" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="291" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="291" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="292" t="s">
+        <v>336</v>
+      </c>
+      <c r="H12" s="293"/>
+      <c r="I12" s="293"/>
+      <c r="J12" s="294"/>
+      <c r="K12" s="295" t="s">
+        <v>138</v>
+      </c>
+      <c r="L12" s="296"/>
+      <c r="M12" s="296"/>
+      <c r="N12" s="297"/>
       <c r="O12" s="288"/>
       <c r="P12" s="289"/>
     </row>
     <row r="13" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="230" t="s">
+      <c r="A13" s="231" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="20" t="s">
@@ -5002,7 +4999,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="230"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="21" t="s">
         <v>9</v>
       </c>
@@ -5042,7 +5039,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="230"/>
+      <c r="A15" s="231"/>
       <c r="B15" s="21" t="s">
         <v>10</v>
       </c>
@@ -5058,7 +5055,7 @@
       <c r="F15" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="277" t="s">
+      <c r="G15" s="244" t="s">
         <v>302</v>
       </c>
       <c r="H15" s="11" t="s">
@@ -5082,7 +5079,7 @@
       <c r="P15" s="55"/>
     </row>
     <row r="16" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="230"/>
+      <c r="A16" s="231"/>
       <c r="B16" s="21" t="s">
         <v>11</v>
       </c>
@@ -5098,7 +5095,7 @@
       <c r="F16" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="278"/>
+      <c r="G16" s="245"/>
       <c r="H16" s="11" t="s">
         <v>86</v>
       </c>
@@ -5120,7 +5117,7 @@
       <c r="P16" s="55"/>
     </row>
     <row r="17" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="230"/>
+      <c r="A17" s="231"/>
       <c r="B17" s="21" t="s">
         <v>12</v>
       </c>
@@ -5136,7 +5133,7 @@
       <c r="F17" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="278"/>
+      <c r="G17" s="245"/>
       <c r="H17" s="11" t="s">
         <v>86</v>
       </c>
@@ -5158,7 +5155,7 @@
       <c r="P17" s="55"/>
     </row>
     <row r="18" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="230"/>
+      <c r="A18" s="231"/>
       <c r="B18" s="21" t="s">
         <v>13</v>
       </c>
@@ -5174,7 +5171,7 @@
       <c r="F18" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="278"/>
+      <c r="G18" s="245"/>
       <c r="H18" s="11" t="s">
         <v>86</v>
       </c>
@@ -5196,7 +5193,7 @@
       <c r="P18" s="55"/>
     </row>
     <row r="19" spans="1:16" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="230"/>
+      <c r="A19" s="231"/>
       <c r="B19" s="21" t="s">
         <v>14</v>
       </c>
@@ -5212,7 +5209,7 @@
       <c r="F19" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="278"/>
+      <c r="G19" s="245"/>
       <c r="H19" s="11" t="s">
         <v>86</v>
       </c>
@@ -5234,7 +5231,7 @@
       <c r="P19" s="55"/>
     </row>
     <row r="20" spans="1:16" ht="219.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="230"/>
+      <c r="A20" s="231"/>
       <c r="B20" s="21" t="s">
         <v>15</v>
       </c>
@@ -5250,7 +5247,7 @@
       <c r="F20" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="279"/>
+      <c r="G20" s="246"/>
       <c r="H20" s="11" t="s">
         <v>86</v>
       </c>
@@ -5272,7 +5269,7 @@
       <c r="P20" s="55"/>
     </row>
     <row r="21" spans="1:16" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="230"/>
+      <c r="A21" s="231"/>
       <c r="B21" s="21" t="s">
         <v>16</v>
       </c>
@@ -5312,7 +5309,7 @@
       <c r="P21" s="55"/>
     </row>
     <row r="22" spans="1:16" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="230"/>
+      <c r="A22" s="231"/>
       <c r="B22" s="21" t="s">
         <v>17</v>
       </c>
@@ -5352,7 +5349,7 @@
       <c r="P22" s="55"/>
     </row>
     <row r="23" spans="1:16" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="230"/>
+      <c r="A23" s="231"/>
       <c r="B23" s="21" t="s">
         <v>18</v>
       </c>
@@ -5390,7 +5387,7 @@
       <c r="P23" s="55"/>
     </row>
     <row r="24" spans="1:16" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="231"/>
+      <c r="A24" s="232"/>
       <c r="B24" s="22" t="s">
         <v>19</v>
       </c>
@@ -5428,7 +5425,7 @@
       <c r="P24" s="57"/>
     </row>
     <row r="25" spans="1:16" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="232" t="s">
+      <c r="A25" s="233" t="s">
         <v>20</v>
       </c>
       <c r="B25" s="38" t="s">
@@ -5468,7 +5465,7 @@
       <c r="P25" s="59"/>
     </row>
     <row r="26" spans="1:16" ht="167.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="233"/>
+      <c r="A26" s="234"/>
       <c r="B26" s="18" t="s">
         <v>93</v>
       </c>
@@ -5508,7 +5505,7 @@
       <c r="P26" s="61"/>
     </row>
     <row r="27" spans="1:16" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="233"/>
+      <c r="A27" s="234"/>
       <c r="B27" s="18" t="s">
         <v>92</v>
       </c>
@@ -5548,7 +5545,7 @@
       <c r="P27" s="61"/>
     </row>
     <row r="28" spans="1:16" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="234"/>
+      <c r="A28" s="235"/>
       <c r="B28" s="19" t="s">
         <v>21</v>
       </c>
@@ -5588,7 +5585,7 @@
       <c r="P28" s="63"/>
     </row>
     <row r="29" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="219" t="s">
+      <c r="A29" s="220" t="s">
         <v>22</v>
       </c>
       <c r="B29" s="6" t="s">
@@ -5606,7 +5603,7 @@
       <c r="F29" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="G29" s="272" t="s">
+      <c r="G29" s="241" t="s">
         <v>310</v>
       </c>
       <c r="H29" s="3"/>
@@ -5624,7 +5621,7 @@
       <c r="P29" s="59"/>
     </row>
     <row r="30" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="220"/>
+      <c r="A30" s="221"/>
       <c r="B30" s="4" t="s">
         <v>104</v>
       </c>
@@ -5640,7 +5637,7 @@
       <c r="F30" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G30" s="273"/>
+      <c r="G30" s="242"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -5656,7 +5653,7 @@
       <c r="P30" s="61"/>
     </row>
     <row r="31" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="220"/>
+      <c r="A31" s="221"/>
       <c r="B31" s="51" t="s">
         <v>106</v>
       </c>
@@ -5672,7 +5669,7 @@
       <c r="F31" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G31" s="273"/>
+      <c r="G31" s="242"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -5688,7 +5685,7 @@
       <c r="P31" s="61"/>
     </row>
     <row r="32" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="220"/>
+      <c r="A32" s="221"/>
       <c r="B32" s="4" t="s">
         <v>105</v>
       </c>
@@ -5704,7 +5701,7 @@
       <c r="F32" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G32" s="273"/>
+      <c r="G32" s="242"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -5720,7 +5717,7 @@
       <c r="P32" s="61"/>
     </row>
     <row r="33" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="220"/>
+      <c r="A33" s="221"/>
       <c r="B33" s="4" t="s">
         <v>107</v>
       </c>
@@ -5736,7 +5733,7 @@
       <c r="F33" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G33" s="273"/>
+      <c r="G33" s="242"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -5752,7 +5749,7 @@
       <c r="P33" s="61"/>
     </row>
     <row r="34" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="220"/>
+      <c r="A34" s="221"/>
       <c r="B34" s="4" t="s">
         <v>109</v>
       </c>
@@ -5768,7 +5765,7 @@
       <c r="F34" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G34" s="276"/>
+      <c r="G34" s="247"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -5784,7 +5781,7 @@
       <c r="P34" s="61"/>
     </row>
     <row r="35" spans="1:16" ht="262.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="220"/>
+      <c r="A35" s="221"/>
       <c r="B35" s="4" t="s">
         <v>24</v>
       </c>
@@ -5818,7 +5815,7 @@
       <c r="P35" s="61"/>
     </row>
     <row r="36" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="220"/>
+      <c r="A36" s="221"/>
       <c r="B36" s="4" t="s">
         <v>25</v>
       </c>
@@ -5860,7 +5857,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" ht="176.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="221"/>
+      <c r="A37" s="222"/>
       <c r="B37" s="5" t="s">
         <v>26</v>
       </c>
@@ -5900,7 +5897,7 @@
       <c r="P37" s="63"/>
     </row>
     <row r="38" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="217" t="s">
+      <c r="A38" s="218" t="s">
         <v>108</v>
       </c>
       <c r="B38" s="44" t="s">
@@ -5936,7 +5933,7 @@
       <c r="P38" s="59"/>
     </row>
     <row r="39" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="218"/>
+      <c r="A39" s="219"/>
       <c r="B39" s="45" t="s">
         <v>28</v>
       </c>
@@ -5976,7 +5973,7 @@
       <c r="P39" s="61"/>
     </row>
     <row r="40" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="218"/>
+      <c r="A40" s="219"/>
       <c r="B40" s="45" t="s">
         <v>29</v>
       </c>
@@ -6014,7 +6011,7 @@
       <c r="P40" s="61"/>
     </row>
     <row r="41" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="218"/>
+      <c r="A41" s="219"/>
       <c r="B41" s="45" t="s">
         <v>30</v>
       </c>
@@ -6054,7 +6051,7 @@
       <c r="P41" s="61"/>
     </row>
     <row r="42" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="218"/>
+      <c r="A42" s="219"/>
       <c r="B42" s="45" t="s">
         <v>31</v>
       </c>
@@ -6070,7 +6067,7 @@
       <c r="F42" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G42" s="275" t="s">
+      <c r="G42" s="248" t="s">
         <v>317</v>
       </c>
       <c r="H42" s="14" t="s">
@@ -6092,7 +6089,7 @@
       <c r="P42" s="61"/>
     </row>
     <row r="43" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="218"/>
+      <c r="A43" s="219"/>
       <c r="B43" s="45" t="s">
         <v>32</v>
       </c>
@@ -6108,7 +6105,7 @@
       <c r="F43" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G43" s="273"/>
+      <c r="G43" s="242"/>
       <c r="H43" s="14" t="s">
         <v>77</v>
       </c>
@@ -6128,7 +6125,7 @@
       <c r="P43" s="61"/>
     </row>
     <row r="44" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="218"/>
+      <c r="A44" s="219"/>
       <c r="B44" s="45" t="s">
         <v>33</v>
       </c>
@@ -6144,7 +6141,7 @@
       <c r="F44" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G44" s="276"/>
+      <c r="G44" s="247"/>
       <c r="H44" s="14" t="s">
         <v>77</v>
       </c>
@@ -6164,7 +6161,7 @@
       <c r="P44" s="61"/>
     </row>
     <row r="45" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="218"/>
+      <c r="A45" s="219"/>
       <c r="B45" s="45" t="s">
         <v>34</v>
       </c>
@@ -6204,7 +6201,7 @@
       <c r="P45" s="61"/>
     </row>
     <row r="46" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="218"/>
+      <c r="A46" s="219"/>
       <c r="B46" s="45" t="s">
         <v>35</v>
       </c>
@@ -6244,7 +6241,7 @@
       <c r="P46" s="61"/>
     </row>
     <row r="47" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="218"/>
+      <c r="A47" s="219"/>
       <c r="B47" s="45" t="s">
         <v>36</v>
       </c>
@@ -6284,7 +6281,7 @@
       <c r="P47" s="61"/>
     </row>
     <row r="48" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="218"/>
+      <c r="A48" s="219"/>
       <c r="B48" s="45" t="s">
         <v>37</v>
       </c>
@@ -6324,7 +6321,7 @@
       <c r="P48" s="61"/>
     </row>
     <row r="49" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="218"/>
+      <c r="A49" s="219"/>
       <c r="B49" s="45" t="s">
         <v>120</v>
       </c>
@@ -6364,7 +6361,7 @@
       <c r="P49" s="61"/>
     </row>
     <row r="50" spans="1:16" ht="146.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="218"/>
+      <c r="A50" s="219"/>
       <c r="B50" s="208" t="s">
         <v>38</v>
       </c>
@@ -6404,7 +6401,7 @@
       <c r="P50" s="63"/>
     </row>
     <row r="51" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="235" t="s">
+      <c r="A51" s="236" t="s">
         <v>39</v>
       </c>
       <c r="B51" s="215" t="s">
@@ -6446,7 +6443,7 @@
       <c r="P51" s="59"/>
     </row>
     <row r="52" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="236"/>
+      <c r="A52" s="237"/>
       <c r="B52" s="214" t="s">
         <v>41</v>
       </c>
@@ -6486,7 +6483,7 @@
       <c r="P52" s="61"/>
     </row>
     <row r="53" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="236"/>
+      <c r="A53" s="237"/>
       <c r="B53" s="214" t="s">
         <v>42</v>
       </c>
@@ -6526,7 +6523,7 @@
       <c r="P53" s="61"/>
     </row>
     <row r="54" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="236"/>
+      <c r="A54" s="237"/>
       <c r="B54" s="214" t="s">
         <v>43</v>
       </c>
@@ -6562,7 +6559,7 @@
       <c r="P54" s="61"/>
     </row>
     <row r="55" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="236"/>
+      <c r="A55" s="237"/>
       <c r="B55" s="214" t="s">
         <v>44</v>
       </c>
@@ -6602,7 +6599,7 @@
       <c r="P55" s="61"/>
     </row>
     <row r="56" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="236"/>
+      <c r="A56" s="237"/>
       <c r="B56" s="214" t="s">
         <v>45</v>
       </c>
@@ -6642,7 +6639,7 @@
       <c r="P56" s="61"/>
     </row>
     <row r="57" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="236"/>
+      <c r="A57" s="237"/>
       <c r="B57" s="214" t="s">
         <v>46</v>
       </c>
@@ -6678,7 +6675,7 @@
       <c r="P57" s="61"/>
     </row>
     <row r="58" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="236"/>
+      <c r="A58" s="237"/>
       <c r="B58" s="214" t="s">
         <v>47</v>
       </c>
@@ -6718,7 +6715,7 @@
       <c r="P58" s="61"/>
     </row>
     <row r="59" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="236"/>
+      <c r="A59" s="237"/>
       <c r="B59" s="214" t="s">
         <v>48</v>
       </c>
@@ -6758,7 +6755,7 @@
       <c r="P59" s="61"/>
     </row>
     <row r="60" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="236"/>
+      <c r="A60" s="237"/>
       <c r="B60" s="214" t="s">
         <v>49</v>
       </c>
@@ -6798,7 +6795,7 @@
       <c r="P60" s="61"/>
     </row>
     <row r="61" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="236"/>
+      <c r="A61" s="237"/>
       <c r="B61" s="214" t="s">
         <v>50</v>
       </c>
@@ -6838,7 +6835,7 @@
       <c r="P61" s="61"/>
     </row>
     <row r="62" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="236"/>
+      <c r="A62" s="237"/>
       <c r="B62" s="214" t="s">
         <v>51</v>
       </c>
@@ -6878,7 +6875,7 @@
       <c r="P62" s="61"/>
     </row>
     <row r="63" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="236"/>
+      <c r="A63" s="237"/>
       <c r="B63" s="214" t="s">
         <v>52</v>
       </c>
@@ -6918,7 +6915,7 @@
       <c r="P63" s="61"/>
     </row>
     <row r="64" spans="1:16" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="237"/>
+      <c r="A64" s="238"/>
       <c r="B64" s="216" t="s">
         <v>53</v>
       </c>
@@ -6958,7 +6955,7 @@
       <c r="P64" s="61"/>
     </row>
     <row r="65" spans="1:16" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="225" t="s">
+      <c r="A65" s="226" t="s">
         <v>54</v>
       </c>
       <c r="B65" s="209" t="s">
@@ -7000,7 +6997,7 @@
       <c r="P65" s="93"/>
     </row>
     <row r="66" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="225"/>
+      <c r="A66" s="226"/>
       <c r="B66" s="71" t="s">
         <v>56</v>
       </c>
@@ -7040,7 +7037,7 @@
       </c>
     </row>
     <row r="67" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="225"/>
+      <c r="A67" s="226"/>
       <c r="B67" s="71" t="s">
         <v>57</v>
       </c>
@@ -7078,7 +7075,7 @@
       <c r="P67" s="95"/>
     </row>
     <row r="68" spans="1:16" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="226"/>
+      <c r="A68" s="227"/>
       <c r="B68" s="72" t="s">
         <v>58</v>
       </c>
@@ -7182,28 +7179,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="240" t="s">
+      <c r="F1" s="249" t="s">
         <v>186</v>
       </c>
-      <c r="G1" s="241"/>
-      <c r="H1" s="241"/>
-      <c r="I1" s="241"/>
-      <c r="J1" s="241"/>
-      <c r="K1" s="241"/>
-      <c r="L1" s="241"/>
-      <c r="M1" s="241"/>
-      <c r="N1" s="241"/>
-      <c r="O1" s="241"/>
-      <c r="P1" s="241"/>
-      <c r="Q1" s="241"/>
-      <c r="R1" s="241"/>
-      <c r="S1" s="241"/>
-      <c r="T1" s="241"/>
-      <c r="U1" s="241"/>
-      <c r="V1" s="241"/>
-      <c r="W1" s="241"/>
-      <c r="X1" s="241"/>
-      <c r="Y1" s="242"/>
+      <c r="G1" s="250"/>
+      <c r="H1" s="250"/>
+      <c r="I1" s="250"/>
+      <c r="J1" s="250"/>
+      <c r="K1" s="250"/>
+      <c r="L1" s="250"/>
+      <c r="M1" s="250"/>
+      <c r="N1" s="250"/>
+      <c r="O1" s="250"/>
+      <c r="P1" s="250"/>
+      <c r="Q1" s="250"/>
+      <c r="R1" s="250"/>
+      <c r="S1" s="250"/>
+      <c r="T1" s="250"/>
+      <c r="U1" s="250"/>
+      <c r="V1" s="250"/>
+      <c r="W1" s="250"/>
+      <c r="X1" s="250"/>
+      <c r="Y1" s="251"/>
     </row>
     <row r="2" spans="1:27" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="103" t="s">
@@ -7289,7 +7286,7 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="249" t="s">
+      <c r="A3" s="258" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="146" t="s">
@@ -7373,7 +7370,7 @@
       </c>
     </row>
     <row r="4" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="250"/>
+      <c r="A4" s="259"/>
       <c r="B4" s="144" t="s">
         <v>3</v>
       </c>
@@ -7453,7 +7450,7 @@
       </c>
     </row>
     <row r="5" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="250"/>
+      <c r="A5" s="259"/>
       <c r="B5" s="144" t="s">
         <v>68</v>
       </c>
@@ -7531,7 +7528,7 @@
       </c>
     </row>
     <row r="6" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="250"/>
+      <c r="A6" s="259"/>
       <c r="B6" s="144" t="s">
         <v>69</v>
       </c>
@@ -7609,7 +7606,7 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="250"/>
+      <c r="A7" s="259"/>
       <c r="B7" s="144" t="s">
         <v>4</v>
       </c>
@@ -7689,7 +7686,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="251"/>
+      <c r="A8" s="260"/>
       <c r="B8" s="159" t="s">
         <v>70</v>
       </c>
@@ -7769,7 +7766,7 @@
       </c>
     </row>
     <row r="9" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="252" t="s">
+      <c r="A9" s="261" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="128" t="s">
@@ -7849,7 +7846,7 @@
       </c>
     </row>
     <row r="10" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="253"/>
+      <c r="A10" s="262"/>
       <c r="B10" s="127" t="s">
         <v>75</v>
       </c>
@@ -7927,7 +7924,7 @@
       </c>
     </row>
     <row r="11" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="253"/>
+      <c r="A11" s="262"/>
       <c r="B11" s="127" t="s">
         <v>111</v>
       </c>
@@ -8005,7 +8002,7 @@
       </c>
     </row>
     <row r="12" spans="1:27" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="254"/>
+      <c r="A12" s="263"/>
       <c r="B12" s="176" t="s">
         <v>76</v>
       </c>
@@ -8083,7 +8080,7 @@
       </c>
     </row>
     <row r="13" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="255" t="s">
+      <c r="A13" s="264" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="178" t="s">
@@ -8163,7 +8160,7 @@
       </c>
     </row>
     <row r="14" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="256"/>
+      <c r="A14" s="265"/>
       <c r="B14" s="177" t="s">
         <v>9</v>
       </c>
@@ -8241,7 +8238,7 @@
       </c>
     </row>
     <row r="15" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="256"/>
+      <c r="A15" s="265"/>
       <c r="B15" s="177" t="s">
         <v>10</v>
       </c>
@@ -8319,7 +8316,7 @@
       </c>
     </row>
     <row r="16" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="256"/>
+      <c r="A16" s="265"/>
       <c r="B16" s="177" t="s">
         <v>11</v>
       </c>
@@ -8397,7 +8394,7 @@
       </c>
     </row>
     <row r="17" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="256"/>
+      <c r="A17" s="265"/>
       <c r="B17" s="177" t="s">
         <v>12</v>
       </c>
@@ -8475,7 +8472,7 @@
       </c>
     </row>
     <row r="18" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="256"/>
+      <c r="A18" s="265"/>
       <c r="B18" s="177" t="s">
         <v>13</v>
       </c>
@@ -8553,7 +8550,7 @@
       </c>
     </row>
     <row r="19" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="256"/>
+      <c r="A19" s="265"/>
       <c r="B19" s="177" t="s">
         <v>14</v>
       </c>
@@ -8631,7 +8628,7 @@
       </c>
     </row>
     <row r="20" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="256"/>
+      <c r="A20" s="265"/>
       <c r="B20" s="177" t="s">
         <v>15</v>
       </c>
@@ -8709,7 +8706,7 @@
       </c>
     </row>
     <row r="21" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="256"/>
+      <c r="A21" s="265"/>
       <c r="B21" s="177" t="s">
         <v>16</v>
       </c>
@@ -8787,7 +8784,7 @@
       </c>
     </row>
     <row r="22" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="256"/>
+      <c r="A22" s="265"/>
       <c r="B22" s="177" t="s">
         <v>17</v>
       </c>
@@ -8865,7 +8862,7 @@
       </c>
     </row>
     <row r="23" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="256"/>
+      <c r="A23" s="265"/>
       <c r="B23" s="177" t="s">
         <v>18</v>
       </c>
@@ -8943,7 +8940,7 @@
       </c>
     </row>
     <row r="24" spans="1:27" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="257"/>
+      <c r="A24" s="266"/>
       <c r="B24" s="180" t="s">
         <v>19</v>
       </c>
@@ -9021,7 +9018,7 @@
       </c>
     </row>
     <row r="25" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="258" t="s">
+      <c r="A25" s="267" t="s">
         <v>20</v>
       </c>
       <c r="B25" s="150" t="s">
@@ -9101,7 +9098,7 @@
       </c>
     </row>
     <row r="26" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="259"/>
+      <c r="A26" s="268"/>
       <c r="B26" s="149" t="s">
         <v>93</v>
       </c>
@@ -9179,7 +9176,7 @@
       </c>
     </row>
     <row r="27" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="259"/>
+      <c r="A27" s="268"/>
       <c r="B27" s="149" t="s">
         <v>92</v>
       </c>
@@ -9257,7 +9254,7 @@
       </c>
     </row>
     <row r="28" spans="1:27" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="260"/>
+      <c r="A28" s="269"/>
       <c r="B28" s="151" t="s">
         <v>21</v>
       </c>
@@ -9335,7 +9332,7 @@
       </c>
     </row>
     <row r="29" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="261" t="s">
+      <c r="A29" s="270" t="s">
         <v>22</v>
       </c>
       <c r="B29" s="154" t="s">
@@ -9415,7 +9412,7 @@
       </c>
     </row>
     <row r="30" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="262"/>
+      <c r="A30" s="271"/>
       <c r="B30" s="153" t="s">
         <v>104</v>
       </c>
@@ -9493,7 +9490,7 @@
       </c>
     </row>
     <row r="31" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="262"/>
+      <c r="A31" s="271"/>
       <c r="B31" s="153" t="s">
         <v>106</v>
       </c>
@@ -9571,7 +9568,7 @@
       </c>
     </row>
     <row r="32" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="262"/>
+      <c r="A32" s="271"/>
       <c r="B32" s="153" t="s">
         <v>105</v>
       </c>
@@ -9649,7 +9646,7 @@
       </c>
     </row>
     <row r="33" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="262"/>
+      <c r="A33" s="271"/>
       <c r="B33" s="153" t="s">
         <v>107</v>
       </c>
@@ -9727,7 +9724,7 @@
       </c>
     </row>
     <row r="34" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="262"/>
+      <c r="A34" s="271"/>
       <c r="B34" s="153" t="s">
         <v>109</v>
       </c>
@@ -9805,7 +9802,7 @@
       </c>
     </row>
     <row r="35" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="262"/>
+      <c r="A35" s="271"/>
       <c r="B35" s="153" t="s">
         <v>24</v>
       </c>
@@ -9883,7 +9880,7 @@
       </c>
     </row>
     <row r="36" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="262"/>
+      <c r="A36" s="271"/>
       <c r="B36" s="153" t="s">
         <v>25</v>
       </c>
@@ -9961,7 +9958,7 @@
       </c>
     </row>
     <row r="37" spans="1:27" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="263"/>
+      <c r="A37" s="272"/>
       <c r="B37" s="188" t="s">
         <v>26</v>
       </c>
@@ -10039,7 +10036,7 @@
       </c>
     </row>
     <row r="38" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="264" t="s">
+      <c r="A38" s="273" t="s">
         <v>108</v>
       </c>
       <c r="B38" s="183" t="s">
@@ -10119,7 +10116,7 @@
       </c>
     </row>
     <row r="39" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="265"/>
+      <c r="A39" s="274"/>
       <c r="B39" s="162" t="s">
         <v>28</v>
       </c>
@@ -10197,7 +10194,7 @@
       </c>
     </row>
     <row r="40" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="265"/>
+      <c r="A40" s="274"/>
       <c r="B40" s="162" t="s">
         <v>29</v>
       </c>
@@ -10275,7 +10272,7 @@
       </c>
     </row>
     <row r="41" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="265"/>
+      <c r="A41" s="274"/>
       <c r="B41" s="162" t="s">
         <v>30</v>
       </c>
@@ -10353,7 +10350,7 @@
       </c>
     </row>
     <row r="42" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="265"/>
+      <c r="A42" s="274"/>
       <c r="B42" s="162" t="s">
         <v>31</v>
       </c>
@@ -10431,7 +10428,7 @@
       </c>
     </row>
     <row r="43" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="265"/>
+      <c r="A43" s="274"/>
       <c r="B43" s="162" t="s">
         <v>32</v>
       </c>
@@ -10509,7 +10506,7 @@
       </c>
     </row>
     <row r="44" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="265"/>
+      <c r="A44" s="274"/>
       <c r="B44" s="162" t="s">
         <v>33</v>
       </c>
@@ -10587,7 +10584,7 @@
       </c>
     </row>
     <row r="45" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="265"/>
+      <c r="A45" s="274"/>
       <c r="B45" s="162" t="s">
         <v>34</v>
       </c>
@@ -10665,7 +10662,7 @@
       </c>
     </row>
     <row r="46" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="265"/>
+      <c r="A46" s="274"/>
       <c r="B46" s="162" t="s">
         <v>35</v>
       </c>
@@ -10743,7 +10740,7 @@
       </c>
     </row>
     <row r="47" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="265"/>
+      <c r="A47" s="274"/>
       <c r="B47" s="162" t="s">
         <v>36</v>
       </c>
@@ -10821,7 +10818,7 @@
       </c>
     </row>
     <row r="48" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="265"/>
+      <c r="A48" s="274"/>
       <c r="B48" s="162" t="s">
         <v>37</v>
       </c>
@@ -10899,7 +10896,7 @@
       </c>
     </row>
     <row r="49" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="265"/>
+      <c r="A49" s="274"/>
       <c r="B49" s="162" t="s">
         <v>120</v>
       </c>
@@ -10977,7 +10974,7 @@
       </c>
     </row>
     <row r="50" spans="1:27" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="266"/>
+      <c r="A50" s="275"/>
       <c r="B50" s="163" t="s">
         <v>38</v>
       </c>
@@ -11055,7 +11052,7 @@
       </c>
     </row>
     <row r="51" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="243" t="s">
+      <c r="A51" s="252" t="s">
         <v>39</v>
       </c>
       <c r="B51" s="165" t="s">
@@ -11135,7 +11132,7 @@
       </c>
     </row>
     <row r="52" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="244"/>
+      <c r="A52" s="253"/>
       <c r="B52" s="164" t="s">
         <v>41</v>
       </c>
@@ -11213,7 +11210,7 @@
       </c>
     </row>
     <row r="53" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="244"/>
+      <c r="A53" s="253"/>
       <c r="B53" s="164" t="s">
         <v>42</v>
       </c>
@@ -11291,7 +11288,7 @@
       </c>
     </row>
     <row r="54" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="244"/>
+      <c r="A54" s="253"/>
       <c r="B54" s="164" t="s">
         <v>43</v>
       </c>
@@ -11369,7 +11366,7 @@
       </c>
     </row>
     <row r="55" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="244"/>
+      <c r="A55" s="253"/>
       <c r="B55" s="164" t="s">
         <v>44</v>
       </c>
@@ -11447,7 +11444,7 @@
       </c>
     </row>
     <row r="56" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="244"/>
+      <c r="A56" s="253"/>
       <c r="B56" s="164" t="s">
         <v>45</v>
       </c>
@@ -11525,7 +11522,7 @@
       </c>
     </row>
     <row r="57" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="244"/>
+      <c r="A57" s="253"/>
       <c r="B57" s="164" t="s">
         <v>46</v>
       </c>
@@ -11603,7 +11600,7 @@
       </c>
     </row>
     <row r="58" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="244"/>
+      <c r="A58" s="253"/>
       <c r="B58" s="164" t="s">
         <v>47</v>
       </c>
@@ -11681,7 +11678,7 @@
       </c>
     </row>
     <row r="59" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="244"/>
+      <c r="A59" s="253"/>
       <c r="B59" s="164" t="s">
         <v>48</v>
       </c>
@@ -11759,7 +11756,7 @@
       </c>
     </row>
     <row r="60" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="244"/>
+      <c r="A60" s="253"/>
       <c r="B60" s="164" t="s">
         <v>49</v>
       </c>
@@ -11833,7 +11830,7 @@
       </c>
     </row>
     <row r="61" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="244"/>
+      <c r="A61" s="253"/>
       <c r="B61" s="164" t="s">
         <v>50</v>
       </c>
@@ -11907,7 +11904,7 @@
       </c>
     </row>
     <row r="62" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="244"/>
+      <c r="A62" s="253"/>
       <c r="B62" s="164" t="s">
         <v>51</v>
       </c>
@@ -11985,7 +11982,7 @@
       </c>
     </row>
     <row r="63" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="244"/>
+      <c r="A63" s="253"/>
       <c r="B63" s="164" t="s">
         <v>52</v>
       </c>
@@ -12063,7 +12060,7 @@
       </c>
     </row>
     <row r="64" spans="1:27" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="245"/>
+      <c r="A64" s="254"/>
       <c r="B64" s="166" t="s">
         <v>53</v>
       </c>
@@ -12141,7 +12138,7 @@
       </c>
     </row>
     <row r="65" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="246" t="s">
+      <c r="A65" s="255" t="s">
         <v>54</v>
       </c>
       <c r="B65" s="169" t="s">
@@ -12221,7 +12218,7 @@
       </c>
     </row>
     <row r="66" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="247"/>
+      <c r="A66" s="256"/>
       <c r="B66" s="168" t="s">
         <v>56</v>
       </c>
@@ -12299,7 +12296,7 @@
       </c>
     </row>
     <row r="67" spans="1:27" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="247"/>
+      <c r="A67" s="256"/>
       <c r="B67" s="168" t="s">
         <v>57</v>
       </c>
@@ -12377,7 +12374,7 @@
       </c>
     </row>
     <row r="68" spans="1:27" ht="120" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="248"/>
+      <c r="A68" s="257"/>
       <c r="B68" s="170" t="s">
         <v>58</v>
       </c>
@@ -17010,19 +17007,19 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="268" t="s">
+      <c r="A26" s="277" t="s">
         <v>226</v>
       </c>
-      <c r="B26" s="269"/>
-      <c r="C26" s="270"/>
+      <c r="B26" s="278"/>
+      <c r="C26" s="279"/>
       <c r="D26" s="196"/>
     </row>
     <row r="27" spans="1:8" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="267" t="s">
+      <c r="A27" s="276" t="s">
         <v>227</v>
       </c>
-      <c r="B27" s="267"/>
-      <c r="C27" s="267"/>
+      <c r="B27" s="276"/>
+      <c r="C27" s="276"/>
       <c r="D27" s="197"/>
     </row>
   </sheetData>

</xml_diff>